<commit_message>
Alteração na função de perda, agora temos um parâmetro para compensar os acertos e erros de handicaps
</commit_message>
<xml_diff>
--- a/output_corners_NNNN_AH.xlsx
+++ b/output_corners_NNNN_AH.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA19"/>
+  <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,60 +511,80 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
+          <t>Team 1 -3.5 Odd</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Team 1 +3.5 Odd</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Team 2 -3.5 Odd</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Team 2 +3.5 Odd</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
           <t>Team 1 Over 4.5</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Team 1 Under 4.5</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Team 2 Over 4.5</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Team 2 Under 4.5</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Team 1 Over 5.5</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Team 1 Under 5.5</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Team 2 Over 5.5</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Team 2 Under 5.5</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Team 1 Over 6.5</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Team 1 Under 6.5</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Team 2 Over 6.5</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Team 2 Under 6.5</t>
         </is>
@@ -592,73 +612,85 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1.918722527961089</v>
+        <v>2.312791972610813</v>
       </c>
       <c r="F2" t="n">
-        <v>7.030128039011147</v>
+        <v>6.785086207772856</v>
       </c>
       <c r="G2" t="n">
-        <v>2.971106174752968</v>
+        <v>2.379592068190155</v>
       </c>
       <c r="H2" t="n">
-        <v>2.654800895521396</v>
+        <v>3.397825518057425</v>
       </c>
       <c r="I2" t="n">
-        <v>1.273550938462806</v>
+        <v>1.396083645024922</v>
       </c>
       <c r="J2" t="n">
-        <v>4.655626281596418</v>
+        <v>3.524719241909316</v>
       </c>
       <c r="K2" t="n">
-        <v>1.604302307731661</v>
+        <v>1.417044523243768</v>
       </c>
       <c r="L2" t="n">
-        <v>4.019616389314129</v>
+        <v>5.499148675577953</v>
       </c>
       <c r="M2" t="n">
-        <v>1.14149779036681</v>
+        <v>1.210286789279645</v>
       </c>
       <c r="N2" t="n">
-        <v>8.067248169795882</v>
+        <v>5.755410472648263</v>
       </c>
       <c r="O2" t="n">
-        <v>1.331167893888382</v>
+        <v>1.222264270889324</v>
       </c>
       <c r="P2" t="n">
-        <v>2.445688623481935</v>
+        <v>9.821679661730025</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.69171188301358</v>
+        <v>1.106648910267894</v>
       </c>
       <c r="R2" t="n">
-        <v>3.5589228767841</v>
+        <v>10.37656088081988</v>
       </c>
       <c r="S2" t="n">
-        <v>1.390789425141542</v>
+        <v>1.113357097326734</v>
       </c>
       <c r="T2" t="n">
-        <v>4.068775107818961</v>
+        <v>2.982042807462987</v>
       </c>
       <c r="U2" t="n">
-        <v>1.325862914311345</v>
+        <v>1.5045299709142</v>
       </c>
       <c r="V2" t="n">
-        <v>6.806958390183065</v>
+        <v>3.057572513042207</v>
       </c>
       <c r="W2" t="n">
-        <v>1.172207192269631</v>
+        <v>1.486009602899223</v>
       </c>
       <c r="X2" t="n">
-        <v>7.588487039179724</v>
+        <v>5.351343948514389</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.151779914577247</v>
+        <v>1.229814055572742</v>
       </c>
       <c r="Z2" t="n">
-        <v>14.71913206784491</v>
+        <v>5.537666914872359</v>
       </c>
       <c r="AA2" t="n">
-        <v>1.072890908481289</v>
+        <v>1.220377568199743</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>10.81880282873611</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>1.101845410020187</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>11.30521869351856</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>1.097038212360204</v>
       </c>
     </row>
     <row r="3">
@@ -683,73 +715,85 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1.11552524041357</v>
+        <v>1.175568535820792</v>
       </c>
       <c r="F3" t="n">
-        <v>20.59678246471482</v>
+        <v>15.54541914979087</v>
       </c>
       <c r="G3" t="n">
-        <v>18.17850502717976</v>
+        <v>11.76191966543118</v>
       </c>
       <c r="H3" t="n">
-        <v>1.21497405559426</v>
+        <v>1.31475633059442</v>
       </c>
       <c r="I3" t="n">
-        <v>1.027177263022086</v>
+        <v>1.04607386981364</v>
       </c>
       <c r="J3" t="n">
-        <v>37.7954638841793</v>
+        <v>22.70427628599033</v>
       </c>
       <c r="K3" t="n">
-        <v>5.65172412194424</v>
+        <v>4.177060801641351</v>
       </c>
       <c r="L3" t="n">
-        <v>1.380439985453953</v>
+        <v>1.543038721401227</v>
       </c>
       <c r="M3" t="n">
-        <v>1.011654715015037</v>
+        <v>1.021188018408338</v>
       </c>
       <c r="N3" t="n">
-        <v>86.80218381228732</v>
+        <v>48.19648533090184</v>
       </c>
       <c r="O3" t="n">
-        <v>3.628535480587749</v>
+        <v>2.841489309306812</v>
       </c>
       <c r="P3" t="n">
-        <v>1.181792066493355</v>
+        <v>1.914776842152114</v>
       </c>
       <c r="Q3" t="n">
-        <v>6.50079010206176</v>
+        <v>1.008976212066859</v>
       </c>
       <c r="R3" t="n">
-        <v>6.501423722320078</v>
+        <v>112.4055675770049</v>
       </c>
       <c r="S3" t="n">
-        <v>1.181771128797597</v>
+        <v>2.093162784540313</v>
       </c>
       <c r="T3" t="n">
-        <v>1.376392549725911</v>
+        <v>1.22875781535031</v>
       </c>
       <c r="U3" t="n">
-        <v>3.656800727666367</v>
+        <v>5.371435347328531</v>
       </c>
       <c r="V3" t="n">
-        <v>15.16408165201571</v>
+        <v>4.866051527315383</v>
       </c>
       <c r="W3" t="n">
-        <v>1.070601117994663</v>
+        <v>1.258661839588674</v>
       </c>
       <c r="X3" t="n">
-        <v>1.716532809863553</v>
+        <v>1.468367131900277</v>
       </c>
       <c r="Y3" t="n">
-        <v>2.39560950487449</v>
+        <v>3.13507723298764</v>
       </c>
       <c r="Z3" t="n">
-        <v>40.32104074063835</v>
+        <v>10.34848236615096</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.025431676811303</v>
+        <v>1.106969234238576</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>1.889656460753628</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>2.124029380006863</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>25.00253622135297</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>1.041662263969855</v>
       </c>
     </row>
     <row r="4">
@@ -774,73 +818,85 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3.665326388949124</v>
+        <v>4.008872943892104</v>
       </c>
       <c r="F4" t="n">
-        <v>8.720181207955594</v>
+        <v>8.763026311373036</v>
       </c>
       <c r="G4" t="n">
-        <v>1.632662431452664</v>
+        <v>1.571246184884417</v>
       </c>
       <c r="H4" t="n">
-        <v>5.615049467359925</v>
+        <v>6.336422106173567</v>
       </c>
       <c r="I4" t="n">
-        <v>1.950554092131045</v>
+        <v>2.03688767920148</v>
       </c>
       <c r="J4" t="n">
-        <v>2.052017984329647</v>
+        <v>1.964424614216761</v>
       </c>
       <c r="K4" t="n">
-        <v>1.216682401147058</v>
+        <v>1.187391473182589</v>
       </c>
       <c r="L4" t="n">
-        <v>9.304090138126643</v>
+        <v>10.89053649828339</v>
       </c>
       <c r="M4" t="n">
-        <v>1.572445992203348</v>
+        <v>1.616838986886146</v>
       </c>
       <c r="N4" t="n">
-        <v>2.746889686747555</v>
+        <v>2.621168605194822</v>
       </c>
       <c r="O4" t="n">
-        <v>1.12042258493904</v>
+        <v>1.101106749889004</v>
       </c>
       <c r="P4" t="n">
-        <v>2.198262504909942</v>
+        <v>20.37033672575985</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.83454167672146</v>
+        <v>1.363694527315796</v>
       </c>
       <c r="R4" t="n">
-        <v>1.438510195513642</v>
+        <v>3.749560207519155</v>
       </c>
       <c r="S4" t="n">
-        <v>3.280448687923129</v>
+        <v>1.05162532867434</v>
       </c>
       <c r="T4" t="n">
-        <v>3.5030473068926</v>
+        <v>2.564516363900642</v>
       </c>
       <c r="U4" t="n">
-        <v>1.399513024482724</v>
+        <v>1.639175161777667</v>
       </c>
       <c r="V4" t="n">
-        <v>1.883692515412503</v>
+        <v>1.488167319172882</v>
       </c>
       <c r="W4" t="n">
-        <v>2.131615332888958</v>
+        <v>3.048477972049281</v>
       </c>
       <c r="X4" t="n">
-        <v>6.237820219442979</v>
+        <v>4.346517151790643</v>
       </c>
       <c r="Y4" t="n">
-        <v>1.190919114842461</v>
+        <v>1.29881813080352</v>
       </c>
       <c r="Z4" t="n">
-        <v>2.698821513514658</v>
+        <v>1.983798907094109</v>
       </c>
       <c r="AA4" t="n">
-        <v>1.588643357789318</v>
+        <v>2.016467890733631</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>8.269294338018137</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>1.137564934572815</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>2.90066270798861</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>1.526132277861261</v>
       </c>
     </row>
     <row r="5">
@@ -865,73 +921,85 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1.121283045438992</v>
+        <v>1.17657081177442</v>
       </c>
       <c r="F5" t="n">
-        <v>19.96291216520118</v>
+        <v>15.49871908696802</v>
       </c>
       <c r="G5" t="n">
-        <v>17.22011221324504</v>
+        <v>11.68894169891993</v>
       </c>
       <c r="H5" t="n">
-        <v>1.224138066524888</v>
+        <v>1.316279221522278</v>
       </c>
       <c r="I5" t="n">
-        <v>1.029091634003616</v>
+        <v>1.046452213283515</v>
       </c>
       <c r="J5" t="n">
-        <v>35.3741434350406</v>
+        <v>22.52749953800097</v>
       </c>
       <c r="K5" t="n">
-        <v>5.461535764559488</v>
+        <v>4.161763188827003</v>
       </c>
       <c r="L5" t="n">
-        <v>1.394614110529663</v>
+        <v>1.545311076095041</v>
       </c>
       <c r="M5" t="n">
-        <v>1.012631736073717</v>
+        <v>1.021396912952841</v>
       </c>
       <c r="N5" t="n">
-        <v>80.16568191134904</v>
+        <v>47.73571380151992</v>
       </c>
       <c r="O5" t="n">
-        <v>3.534121242288501</v>
+        <v>2.83381567666106</v>
       </c>
       <c r="P5" t="n">
-        <v>1.181792563053132</v>
+        <v>1.918170088370768</v>
       </c>
       <c r="Q5" t="n">
-        <v>6.500775076853563</v>
+        <v>1.009081668529155</v>
       </c>
       <c r="R5" t="n">
-        <v>6.110813893272541</v>
+        <v>111.1119245642625</v>
       </c>
       <c r="S5" t="n">
-        <v>1.195663552006133</v>
+        <v>2.089122824480628</v>
       </c>
       <c r="T5" t="n">
-        <v>1.376393522379854</v>
+        <v>1.228380907572516</v>
       </c>
       <c r="U5" t="n">
-        <v>3.656793862118613</v>
+        <v>5.378649733154581</v>
       </c>
       <c r="V5" t="n">
-        <v>13.97991600491781</v>
+        <v>4.825515409606563</v>
       </c>
       <c r="W5" t="n">
-        <v>1.077042101013683</v>
+        <v>1.261402685109781</v>
       </c>
       <c r="X5" t="n">
-        <v>1.716534630323189</v>
+        <v>1.467628701235015</v>
       </c>
       <c r="Y5" t="n">
-        <v>2.395605959127134</v>
+        <v>3.138448725150922</v>
       </c>
       <c r="Z5" t="n">
-        <v>36.43558928299527</v>
+        <v>10.23416901756683</v>
       </c>
       <c r="AA5" t="n">
-        <v>1.028220216461304</v>
+        <v>1.108293447747992</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>1.888258338901582</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>2.125798606334051</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>24.65584981744083</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>1.042272841927781</v>
       </c>
     </row>
     <row r="6">
@@ -956,73 +1024,85 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1.116423741964175</v>
+        <v>1.175553945631493</v>
       </c>
       <c r="F6" t="n">
-        <v>20.49397424150552</v>
+        <v>15.54966981035253</v>
       </c>
       <c r="G6" t="n">
-        <v>18.02193964367534</v>
+        <v>11.76094762692905</v>
       </c>
       <c r="H6" t="n">
-        <v>1.216406180927765</v>
+        <v>1.31468454835281</v>
       </c>
       <c r="I6" t="n">
-        <v>1.027474222578841</v>
+        <v>1.046087756948969</v>
       </c>
       <c r="J6" t="n">
-        <v>37.39775419050965</v>
+        <v>22.69773636645521</v>
       </c>
       <c r="K6" t="n">
-        <v>5.62094010306384</v>
+        <v>4.177785516430398</v>
       </c>
       <c r="L6" t="n">
-        <v>1.382656451325532</v>
+        <v>1.542845682779898</v>
       </c>
       <c r="M6" t="n">
-        <v>1.011805586129402</v>
+        <v>1.021199797788762</v>
       </c>
       <c r="N6" t="n">
-        <v>85.7056629835178</v>
+        <v>48.17026124325213</v>
       </c>
       <c r="O6" t="n">
-        <v>3.613310180805716</v>
+        <v>2.842144152052618</v>
       </c>
       <c r="P6" t="n">
-        <v>1.18178770786067</v>
+        <v>1.914340945799745</v>
       </c>
       <c r="Q6" t="n">
-        <v>6.500921991746791</v>
+        <v>1.008983892002674</v>
       </c>
       <c r="R6" t="n">
-        <v>6.436891640760172</v>
+        <v>112.3103318363967</v>
       </c>
       <c r="S6" t="n">
-        <v>1.18392862430861</v>
+        <v>2.093683931135045</v>
       </c>
       <c r="T6" t="n">
-        <v>1.376384012099827</v>
+        <v>1.228330056759684</v>
       </c>
       <c r="U6" t="n">
-        <v>3.656860992636351</v>
+        <v>5.379624891227056</v>
       </c>
       <c r="V6" t="n">
-        <v>14.96708011864893</v>
+        <v>4.857904622083269</v>
       </c>
       <c r="W6" t="n">
-        <v>1.071596925878931</v>
+        <v>1.259208067062062</v>
       </c>
       <c r="X6" t="n">
-        <v>1.716516830495783</v>
+        <v>1.467529076191523</v>
       </c>
       <c r="Y6" t="n">
-        <v>2.3956406289969</v>
+        <v>3.138904403862898</v>
       </c>
       <c r="Z6" t="n">
-        <v>39.66978348722559</v>
+        <v>10.32548648264921</v>
       </c>
       <c r="AA6" t="n">
-        <v>1.025859984458676</v>
+        <v>1.107233011581817</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>1.888069722412551</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>2.126037713889599</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>24.93272400712383</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>1.041783793591667</v>
       </c>
     </row>
     <row r="7">
@@ -1047,73 +1127,85 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1.14240812386288</v>
+        <v>1.571744492928856</v>
       </c>
       <c r="F7" t="n">
-        <v>17.56732446245159</v>
+        <v>7.478886211391416</v>
       </c>
       <c r="G7" t="n">
-        <v>14.76402219104996</v>
+        <v>4.346795635137402</v>
       </c>
       <c r="H7" t="n">
-        <v>1.262655618305185</v>
+        <v>2.064916339067152</v>
       </c>
       <c r="I7" t="n">
-        <v>1.034428543657743</v>
+        <v>1.148811678389527</v>
       </c>
       <c r="J7" t="n">
-        <v>30.04566658238847</v>
+        <v>7.719902704023132</v>
       </c>
       <c r="K7" t="n">
-        <v>4.807266741342191</v>
+        <v>1.939040902382981</v>
       </c>
       <c r="L7" t="n">
-        <v>1.462694849358951</v>
+        <v>2.972962167471333</v>
       </c>
       <c r="M7" t="n">
-        <v>1.015007449644777</v>
+        <v>1.069299347074809</v>
       </c>
       <c r="N7" t="n">
-        <v>67.63357356977886</v>
+        <v>15.43015038684983</v>
       </c>
       <c r="O7" t="n">
-        <v>3.161251635684879</v>
+        <v>1.506852090976311</v>
       </c>
       <c r="P7" t="n">
-        <v>1.229711799731851</v>
+        <v>4.712562281198177</v>
       </c>
       <c r="Q7" t="n">
-        <v>5.353280942325684</v>
+        <v>1.029723651130022</v>
       </c>
       <c r="R7" t="n">
-        <v>6.354799180069366</v>
+        <v>34.64324240066055</v>
       </c>
       <c r="S7" t="n">
-        <v>1.18674836653483</v>
+        <v>1.269355750626563</v>
       </c>
       <c r="T7" t="n">
-        <v>1.470236214576323</v>
+        <v>2.395777500845176</v>
       </c>
       <c r="U7" t="n">
-        <v>3.126590783529904</v>
+        <v>1.716446567876668</v>
       </c>
       <c r="V7" t="n">
-        <v>14.71724479602924</v>
+        <v>6.545201489579058</v>
       </c>
       <c r="W7" t="n">
-        <v>1.07290093709558</v>
+        <v>1.180336098134445</v>
       </c>
       <c r="X7" t="n">
-        <v>1.893195937464387</v>
+        <v>3.953263510630933</v>
       </c>
       <c r="Y7" t="n">
-        <v>2.119575177243651</v>
+        <v>1.338608456847916</v>
       </c>
       <c r="Z7" t="n">
-        <v>38.84661684149125</v>
+        <v>15.29802753557291</v>
       </c>
       <c r="AA7" t="n">
-        <v>1.026422440985629</v>
+        <v>1.069939717035237</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>7.308667115700426</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>1.158512088474488</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>40.76492614841345</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>1.02514778969456</v>
       </c>
     </row>
     <row r="8">
@@ -1138,73 +1230,85 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1.874608754351656</v>
+        <v>1.510373371217801</v>
       </c>
       <c r="F8" t="n">
-        <v>7.058611089641388</v>
+        <v>8.414874654394533</v>
       </c>
       <c r="G8" t="n">
-        <v>3.078017663135952</v>
+        <v>4.564649458239582</v>
       </c>
       <c r="H8" t="n">
-        <v>2.577911426687815</v>
+        <v>1.904803896753523</v>
       </c>
       <c r="I8" t="n">
-        <v>1.257983055838185</v>
+        <v>1.147745297522529</v>
       </c>
       <c r="J8" t="n">
-        <v>4.876223563408093</v>
+        <v>7.768404929080861</v>
       </c>
       <c r="K8" t="n">
-        <v>1.633749133878251</v>
+        <v>2.105211862579334</v>
       </c>
       <c r="L8" t="n">
-        <v>3.87892209902574</v>
+        <v>2.590248612781015</v>
       </c>
       <c r="M8" t="n">
-        <v>1.132377209349239</v>
+        <v>1.073415589581014</v>
       </c>
       <c r="N8" t="n">
-        <v>8.554170426434835</v>
+        <v>14.62108519058491</v>
       </c>
       <c r="O8" t="n">
-        <v>1.347352226146866</v>
+        <v>1.628832493210737</v>
       </c>
       <c r="P8" t="n">
-        <v>2.425676569762615</v>
+        <v>3.817761085606752</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.701421361064037</v>
+        <v>1.033987009466157</v>
       </c>
       <c r="R8" t="n">
-        <v>3.728223762766472</v>
+        <v>30.42300648710465</v>
       </c>
       <c r="S8" t="n">
-        <v>1.366538849799468</v>
+        <v>1.354891692240355</v>
       </c>
       <c r="T8" t="n">
-        <v>4.022377637482552</v>
+        <v>1.773654591072937</v>
       </c>
       <c r="U8" t="n">
-        <v>1.33086533846675</v>
+        <v>2.292566490962275</v>
       </c>
       <c r="V8" t="n">
-        <v>7.247629572583086</v>
+        <v>4.176233839933125</v>
       </c>
       <c r="W8" t="n">
-        <v>1.160060705965727</v>
+        <v>1.314838280301508</v>
       </c>
       <c r="X8" t="n">
-        <v>7.475852077750368</v>
+        <v>2.574991314343375</v>
       </c>
       <c r="Y8" t="n">
-        <v>1.154419833559167</v>
+        <v>1.634924136338433</v>
       </c>
       <c r="Z8" t="n">
-        <v>15.94190895237344</v>
+        <v>8.440795556009052</v>
       </c>
       <c r="AA8" t="n">
-        <v>1.066925852860398</v>
+        <v>1.134394231433011</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>4.142188664816253</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>1.318249509075381</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>19.33903563101921</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>1.054528494306896</v>
       </c>
     </row>
     <row r="9">
@@ -1229,73 +1333,85 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1.115754950513624</v>
+        <v>1.175520022706314</v>
       </c>
       <c r="F9" t="n">
-        <v>20.55415565433699</v>
+        <v>15.55231180122081</v>
       </c>
       <c r="G9" t="n">
-        <v>18.15083230956264</v>
+        <v>11.76283231838263</v>
       </c>
       <c r="H9" t="n">
-        <v>1.215468454267187</v>
+        <v>1.314618381719359</v>
       </c>
       <c r="I9" t="n">
-        <v>1.027208375762801</v>
+        <v>1.046080674037752</v>
       </c>
       <c r="J9" t="n">
-        <v>37.7533883212236</v>
+        <v>22.70107145526457</v>
       </c>
       <c r="K9" t="n">
-        <v>5.641050604836906</v>
+        <v>4.178453828842092</v>
       </c>
       <c r="L9" t="n">
-        <v>1.381422787786976</v>
+        <v>1.542721638142272</v>
       </c>
       <c r="M9" t="n">
-        <v>1.011661272370783</v>
+        <v>1.021197102404618</v>
       </c>
       <c r="N9" t="n">
-        <v>86.7539356087307</v>
+        <v>48.17625932599739</v>
       </c>
       <c r="O9" t="n">
-        <v>3.621762600504342</v>
+        <v>2.842565193131022</v>
       </c>
       <c r="P9" t="n">
-        <v>1.183032582395118</v>
+        <v>1.914112233923191</v>
       </c>
       <c r="Q9" t="n">
-        <v>6.463508119233485</v>
+        <v>1.00898304438841</v>
       </c>
       <c r="R9" t="n">
-        <v>6.531655594770331</v>
+        <v>112.3208347595676</v>
       </c>
       <c r="S9" t="n">
-        <v>1.180777704408316</v>
+        <v>2.093957572045827</v>
       </c>
       <c r="T9" t="n">
-        <v>1.378822390561836</v>
+        <v>1.228215250349452</v>
       </c>
       <c r="U9" t="n">
-        <v>3.639759488653476</v>
+        <v>5.381828113891434</v>
       </c>
       <c r="V9" t="n">
-        <v>15.25655543393986</v>
+        <v>4.856711931340955</v>
       </c>
       <c r="W9" t="n">
-        <v>1.07014317060202</v>
+        <v>1.259288227330037</v>
       </c>
       <c r="X9" t="n">
-        <v>1.721081246271797</v>
+        <v>1.467304152489848</v>
       </c>
       <c r="Y9" t="n">
-        <v>2.386806279001563</v>
+        <v>3.139933905298917</v>
       </c>
       <c r="Z9" t="n">
-        <v>40.62739810314091</v>
+        <v>10.3221208290261</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.025235065834937</v>
+        <v>1.107271726932172</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>1.887643891683332</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>2.126577909643016</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>24.92250935344757</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>1.041801634821218</v>
       </c>
     </row>
     <row r="10">
@@ -1320,73 +1436,85 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2.056836019446762</v>
+        <v>4.263535613010567</v>
       </c>
       <c r="F10" t="n">
-        <v>6.907057294067285</v>
+        <v>8.892132260944718</v>
       </c>
       <c r="G10" t="n">
-        <v>2.709756016385274</v>
+        <v>1.531407841590183</v>
       </c>
       <c r="H10" t="n">
-        <v>2.909676441532259</v>
+        <v>6.857260346271354</v>
       </c>
       <c r="I10" t="n">
-        <v>1.317751903713293</v>
+        <v>2.10754727172351</v>
       </c>
       <c r="J10" t="n">
-        <v>4.147109390420196</v>
+        <v>1.902895998690738</v>
       </c>
       <c r="K10" t="n">
-        <v>1.523648916775469</v>
+        <v>1.170728282658049</v>
       </c>
       <c r="L10" t="n">
-        <v>4.514591384273015</v>
+        <v>12.02012188810848</v>
       </c>
       <c r="M10" t="n">
-        <v>1.166458268376866</v>
+        <v>1.656133303482119</v>
       </c>
       <c r="N10" t="n">
-        <v>7.007511731024225</v>
+        <v>2.524080540787931</v>
       </c>
       <c r="O10" t="n">
-        <v>1.284528097483756</v>
+        <v>1.090743097957843</v>
       </c>
       <c r="P10" t="n">
-        <v>2.61468432613752</v>
+        <v>22.97834288521315</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.61931610025106</v>
+        <v>1.385947942075676</v>
       </c>
       <c r="R10" t="n">
-        <v>3.315245405032524</v>
+        <v>3.591023013678673</v>
       </c>
       <c r="S10" t="n">
-        <v>1.431919656476309</v>
+        <v>1.045499335651588</v>
       </c>
       <c r="T10" t="n">
-        <v>4.464909352517543</v>
+        <v>2.765509237841624</v>
       </c>
       <c r="U10" t="n">
-        <v>1.288607838838097</v>
+        <v>1.566408817674907</v>
       </c>
       <c r="V10" t="n">
-        <v>6.18315650827354</v>
+        <v>1.493782555300931</v>
       </c>
       <c r="W10" t="n">
-        <v>1.192932626750469</v>
+        <v>3.025182925691979</v>
       </c>
       <c r="X10" t="n">
-        <v>8.562818262535936</v>
+        <v>4.824772746352181</v>
       </c>
       <c r="Y10" t="n">
-        <v>1.132225840326445</v>
+        <v>1.261453442156461</v>
       </c>
       <c r="Z10" t="n">
-        <v>13.02033478025395</v>
+        <v>1.995168236546222</v>
       </c>
       <c r="AA10" t="n">
-        <v>1.083192358472638</v>
+        <v>2.00485522274158</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>9.466621393855874</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>1.118110867780823</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>2.923748394645408</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>1.519818497462254</v>
       </c>
     </row>
     <row r="11">
@@ -1411,73 +1539,85 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1.125063063677842</v>
+        <v>1.178969611469527</v>
       </c>
       <c r="F11" t="n">
-        <v>19.5772243901357</v>
+        <v>15.3850369280119</v>
       </c>
       <c r="G11" t="n">
-        <v>16.64414921548259</v>
+        <v>11.52027305145817</v>
       </c>
       <c r="H11" t="n">
-        <v>1.23013414847836</v>
+        <v>1.319978156383952</v>
       </c>
       <c r="I11" t="n">
-        <v>1.030363976596499</v>
+        <v>1.047338049926346</v>
       </c>
       <c r="J11" t="n">
-        <v>33.93376270469434</v>
+        <v>22.1246555689536</v>
       </c>
       <c r="K11" t="n">
-        <v>5.345291677102111</v>
+        <v>4.12521333112523</v>
       </c>
       <c r="L11" t="n">
-        <v>1.403871555074123</v>
+        <v>1.550926604745412</v>
       </c>
       <c r="M11" t="n">
-        <v>1.013286952922467</v>
+        <v>1.021882359864325</v>
       </c>
       <c r="N11" t="n">
-        <v>76.26180049220059</v>
+        <v>46.69891027294187</v>
       </c>
       <c r="O11" t="n">
-        <v>3.476034737867266</v>
+        <v>2.815123813928189</v>
       </c>
       <c r="P11" t="n">
-        <v>1.181793611350487</v>
+        <v>1.92672343389757</v>
       </c>
       <c r="Q11" t="n">
-        <v>6.500743357103248</v>
+        <v>1.009325396862301</v>
       </c>
       <c r="R11" t="n">
-        <v>5.880141303564999</v>
+        <v>108.2340421288221</v>
       </c>
       <c r="S11" t="n">
-        <v>1.204912099424148</v>
+        <v>2.079070587213109</v>
       </c>
       <c r="T11" t="n">
-        <v>1.376395575769127</v>
+        <v>1.227976925784149</v>
       </c>
       <c r="U11" t="n">
-        <v>3.656779368239381</v>
+        <v>5.3864088287023</v>
       </c>
       <c r="V11" t="n">
-        <v>13.29015300723741</v>
+        <v>4.740801488338272</v>
       </c>
       <c r="W11" t="n">
-        <v>1.081365952027702</v>
+        <v>1.267322391502848</v>
       </c>
       <c r="X11" t="n">
-        <v>1.716538473532768</v>
+        <v>1.46683724093097</v>
       </c>
       <c r="Y11" t="n">
-        <v>2.395598473686519</v>
+        <v>3.142074179870039</v>
       </c>
       <c r="Z11" t="n">
-        <v>34.20575740303148</v>
+        <v>9.996135120450173</v>
       </c>
       <c r="AA11" t="n">
-        <v>1.030115259467285</v>
+        <v>1.111158846172373</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>1.886759964560253</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>2.127700888589285</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>23.93680582629139</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>1.043598049683699</v>
       </c>
     </row>
     <row r="12">
@@ -1502,73 +1642,85 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>4.760896333544998</v>
+        <v>2.572616680830862</v>
       </c>
       <c r="F12" t="n">
-        <v>9.367290383855025</v>
+        <v>7.279034277707837</v>
       </c>
       <c r="G12" t="n">
-        <v>1.463697959529252</v>
+        <v>2.110105962872146</v>
       </c>
       <c r="H12" t="n">
-        <v>7.813070193051558</v>
+        <v>3.783863006151783</v>
       </c>
       <c r="I12" t="n">
-        <v>2.267218964622382</v>
+        <v>1.514952608621186</v>
       </c>
       <c r="J12" t="n">
-        <v>1.789129604210107</v>
+        <v>2.941926272939088</v>
       </c>
       <c r="K12" t="n">
-        <v>1.146776705899768</v>
+        <v>1.359213078298106</v>
       </c>
       <c r="L12" t="n">
-        <v>13.98313177068117</v>
+        <v>6.075165128199338</v>
       </c>
       <c r="M12" t="n">
-        <v>1.752518288660609</v>
+        <v>1.289191860407991</v>
       </c>
       <c r="N12" t="n">
-        <v>2.328871357771091</v>
+        <v>4.45791198476058</v>
       </c>
       <c r="O12" t="n">
-        <v>1.077023018610828</v>
+        <v>1.197037923838904</v>
       </c>
       <c r="P12" t="n">
-        <v>2.897776713165366</v>
+        <v>10.66632182911704</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.526932379906836</v>
+        <v>1.15718837056945</v>
       </c>
       <c r="R12" t="n">
-        <v>1.438502444003515</v>
+        <v>7.361793791597162</v>
       </c>
       <c r="S12" t="n">
-        <v>3.280488999947246</v>
+        <v>1.103451966288541</v>
       </c>
       <c r="T12" t="n">
-        <v>5.145067256058605</v>
+        <v>2.507062990172581</v>
       </c>
       <c r="U12" t="n">
-        <v>1.241250609031339</v>
+        <v>1.663542271637555</v>
       </c>
       <c r="V12" t="n">
-        <v>1.883676948995587</v>
+        <v>2.172168523422857</v>
       </c>
       <c r="W12" t="n">
-        <v>2.131635266866052</v>
+        <v>1.85311964962162</v>
       </c>
       <c r="X12" t="n">
-        <v>10.28506316849639</v>
+        <v>4.211752849620511</v>
       </c>
       <c r="Y12" t="n">
-        <v>1.107699859640474</v>
+        <v>1.31135646073083</v>
       </c>
       <c r="Z12" t="n">
-        <v>2.698790328659064</v>
+        <v>3.444414755749374</v>
       </c>
       <c r="AA12" t="n">
-        <v>1.588654163571409</v>
+        <v>1.40909587771386</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>7.937571260544279</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>1.14414266354095</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>6.100786838470794</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>1.196048184656114</v>
       </c>
     </row>
     <row r="13">
@@ -1593,73 +1745,85 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>3.89296489474322</v>
+        <v>2.06457301509098</v>
       </c>
       <c r="F13" t="n">
-        <v>8.569119152445849</v>
+        <v>6.952995651537126</v>
       </c>
       <c r="G13" t="n">
-        <v>1.596351972382697</v>
+        <v>2.68950634220995</v>
       </c>
       <c r="H13" t="n">
-        <v>6.147394408561923</v>
+        <v>2.915418059260459</v>
       </c>
       <c r="I13" t="n">
-        <v>1.988660519010836</v>
+        <v>1.323270044131755</v>
       </c>
       <c r="J13" t="n">
-        <v>2.011469539615589</v>
+        <v>4.093389004495664</v>
       </c>
       <c r="K13" t="n">
-        <v>1.194273047803885</v>
+        <v>1.522079237566601</v>
       </c>
       <c r="L13" t="n">
-        <v>10.56972890134003</v>
+        <v>4.509964855237964</v>
       </c>
       <c r="M13" t="n">
-        <v>1.584704996832931</v>
+        <v>1.17042012987283</v>
       </c>
       <c r="N13" t="n">
-        <v>2.710264159561703</v>
+        <v>6.86785141371627</v>
       </c>
       <c r="O13" t="n">
-        <v>1.104496168105658</v>
+        <v>1.284903137564949</v>
       </c>
       <c r="P13" t="n">
-        <v>2.633401977869857</v>
+        <v>7.662493543578759</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.612219168060586</v>
+        <v>1.085346773752735</v>
       </c>
       <c r="R13" t="n">
-        <v>1.538080308919726</v>
+        <v>12.71690452994945</v>
       </c>
       <c r="S13" t="n">
-        <v>2.858458641624788</v>
+        <v>1.150093954081769</v>
       </c>
       <c r="T13" t="n">
-        <v>4.509250607892016</v>
+        <v>2.551211978700033</v>
       </c>
       <c r="U13" t="n">
-        <v>1.284961124677469</v>
+        <v>1.64465721882707</v>
       </c>
       <c r="V13" t="n">
-        <v>2.085217185174485</v>
+        <v>3.188207299953841</v>
       </c>
       <c r="W13" t="n">
-        <v>1.92147453400235</v>
+        <v>1.456995093664615</v>
       </c>
       <c r="X13" t="n">
-        <v>8.67324764538246</v>
+        <v>4.315231556463168</v>
       </c>
       <c r="Y13" t="n">
-        <v>1.130322914913579</v>
+        <v>1.301638055432497</v>
       </c>
       <c r="Z13" t="n">
-        <v>3.107742030480792</v>
+        <v>5.863046581706702</v>
       </c>
       <c r="AA13" t="n">
-        <v>1.474441362148997</v>
+        <v>1.205632412356833</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>8.192055562825649</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>1.139042307343787</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>12.16410404151427</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>1.08957279476091</v>
       </c>
     </row>
     <row r="14">
@@ -1684,73 +1848,85 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1.118115391208567</v>
+        <v>1.209107988436613</v>
       </c>
       <c r="F14" t="n">
-        <v>20.30384002017952</v>
+        <v>13.76577870776965</v>
       </c>
       <c r="G14" t="n">
-        <v>17.73484868592787</v>
+        <v>9.970079504989293</v>
       </c>
       <c r="H14" t="n">
-        <v>1.219105066576843</v>
+        <v>1.373371774096445</v>
       </c>
       <c r="I14" t="n">
-        <v>1.028033471843295</v>
+        <v>1.055818480942664</v>
       </c>
       <c r="J14" t="n">
-        <v>36.67164301267817</v>
+        <v>18.91521344027933</v>
       </c>
       <c r="K14" t="n">
-        <v>5.5640204292094</v>
+        <v>3.678295654297884</v>
       </c>
       <c r="L14" t="n">
-        <v>1.386839982137999</v>
+        <v>1.644066814925543</v>
       </c>
       <c r="M14" t="n">
-        <v>1.01209006302939</v>
+        <v>1.025959905363033</v>
       </c>
       <c r="N14" t="n">
-        <v>83.71255472937473</v>
+        <v>39.52094166044231</v>
       </c>
       <c r="O14" t="n">
-        <v>3.585048201256677</v>
+        <v>2.552633945463568</v>
       </c>
       <c r="P14" t="n">
-        <v>1.181828925980352</v>
+        <v>2.08954968083223</v>
       </c>
       <c r="Q14" t="n">
-        <v>6.499675008299044</v>
+        <v>1.011129228926067</v>
       </c>
       <c r="R14" t="n">
-        <v>6.320741774961292</v>
+        <v>90.85348460734588</v>
       </c>
       <c r="S14" t="n">
-        <v>1.187943719559154</v>
+        <v>1.91781037394841</v>
       </c>
       <c r="T14" t="n">
-        <v>1.37646474948699</v>
+        <v>1.283337418528626</v>
       </c>
       <c r="U14" t="n">
-        <v>3.656291196885509</v>
+        <v>4.529360877193731</v>
       </c>
       <c r="V14" t="n">
-        <v>14.61385281848415</v>
+        <v>4.833389705771483</v>
       </c>
       <c r="W14" t="n">
-        <v>1.073454591681956</v>
+        <v>1.260865728964216</v>
       </c>
       <c r="X14" t="n">
-        <v>1.716667942504992</v>
+        <v>1.575488024689801</v>
       </c>
       <c r="Y14" t="n">
-        <v>2.395346353158575</v>
+        <v>2.737655619400627</v>
       </c>
       <c r="Z14" t="n">
-        <v>38.50686658897606</v>
+        <v>10.25635402503918</v>
       </c>
       <c r="AA14" t="n">
-        <v>1.026661784652891</v>
+        <v>1.108033897287735</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>2.093965076781798</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>1.914105963000005</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>24.72306273863493</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>1.042153073193683</v>
       </c>
     </row>
     <row r="15">
@@ -1775,73 +1951,85 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>1.214340979348045</v>
+        <v>1.567876903472875</v>
       </c>
       <c r="F15" t="n">
-        <v>13.81877128441145</v>
+        <v>7.613527945879362</v>
       </c>
       <c r="G15" t="n">
-        <v>9.60220620648615</v>
+        <v>4.331823336084757</v>
       </c>
       <c r="H15" t="n">
-        <v>1.377350919886493</v>
+        <v>2.046738966575963</v>
       </c>
       <c r="I15" t="n">
-        <v>1.059437698835846</v>
+        <v>1.15143762728388</v>
       </c>
       <c r="J15" t="n">
-        <v>17.82433909094945</v>
+        <v>7.603378684251528</v>
       </c>
       <c r="K15" t="n">
-        <v>3.650053166163744</v>
+        <v>1.955348020787979</v>
       </c>
       <c r="L15" t="n">
-        <v>1.643171445815543</v>
+        <v>2.918941909316889</v>
       </c>
       <c r="M15" t="n">
-        <v>1.02834783140377</v>
+        <v>1.071621050656204</v>
       </c>
       <c r="N15" t="n">
-        <v>36.27606700338328</v>
+        <v>14.9623754585813</v>
       </c>
       <c r="O15" t="n">
-        <v>2.55479539165797</v>
+        <v>1.521120517064523</v>
       </c>
       <c r="P15" t="n">
-        <v>1.247821134194806</v>
+        <v>4.569431804507134</v>
       </c>
       <c r="Q15" t="n">
-        <v>5.035168361443809</v>
+        <v>1.031287280131874</v>
       </c>
       <c r="R15" t="n">
-        <v>4.149557098749545</v>
+        <v>32.9618706319329</v>
       </c>
       <c r="S15" t="n">
-        <v>1.317504959791656</v>
+        <v>1.280156634099942</v>
       </c>
       <c r="T15" t="n">
-        <v>1.505734294921589</v>
+        <v>2.259483823109361</v>
       </c>
       <c r="U15" t="n">
-        <v>2.977322894732786</v>
+        <v>1.793976057216235</v>
       </c>
       <c r="V15" t="n">
-        <v>8.368692714972134</v>
+        <v>5.903444965526613</v>
       </c>
       <c r="W15" t="n">
-        <v>1.13570928232197</v>
+        <v>1.203938253009964</v>
       </c>
       <c r="X15" t="n">
-        <v>1.960587188906722</v>
+        <v>3.641395563163178</v>
       </c>
       <c r="Y15" t="n">
-        <v>2.041029915398034</v>
+        <v>1.37858774881959</v>
       </c>
       <c r="Z15" t="n">
-        <v>19.13036868138662</v>
+        <v>13.35950594235079</v>
       </c>
       <c r="AA15" t="n">
-        <v>1.055156076391687</v>
+        <v>1.080909383001583</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>6.563428832397946</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>1.179745266835557</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>34.42880524943437</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>1.02991432067459</v>
       </c>
     </row>
     <row r="16">
@@ -1866,73 +2054,85 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>1.368082911990897</v>
+        <v>1.586495278406215</v>
       </c>
       <c r="F16" t="n">
-        <v>10.09877591849138</v>
+        <v>7.537340366629405</v>
       </c>
       <c r="G16" t="n">
-        <v>5.881375683959416</v>
+        <v>4.219284304326422</v>
       </c>
       <c r="H16" t="n">
-        <v>1.639856291065558</v>
+        <v>2.080255361250555</v>
       </c>
       <c r="I16" t="n">
-        <v>1.108731122867891</v>
+        <v>1.157275898661488</v>
       </c>
       <c r="J16" t="n">
-        <v>10.19699873986413</v>
+        <v>7.358253289350733</v>
       </c>
       <c r="K16" t="n">
-        <v>2.562850930690535</v>
+        <v>1.925707046565687</v>
       </c>
       <c r="L16" t="n">
-        <v>2.092377872157176</v>
+        <v>2.981502624941098</v>
       </c>
       <c r="M16" t="n">
-        <v>1.054330554110539</v>
+        <v>1.074737270284719</v>
       </c>
       <c r="N16" t="n">
-        <v>19.40584945931966</v>
+        <v>14.38020503278224</v>
       </c>
       <c r="O16" t="n">
-        <v>1.915434141873681</v>
+        <v>1.504667512125918</v>
       </c>
       <c r="P16" t="n">
-        <v>1.437844248571184</v>
+        <v>4.692417989205637</v>
       </c>
       <c r="Q16" t="n">
-        <v>3.283917176629124</v>
+        <v>1.032841377350513</v>
       </c>
       <c r="R16" t="n">
-        <v>3.693532516309961</v>
+        <v>31.44939282926833</v>
       </c>
       <c r="S16" t="n">
-        <v>1.371259672547025</v>
+        <v>1.270825243220943</v>
       </c>
       <c r="T16" t="n">
-        <v>1.88235524256844</v>
+        <v>2.287094708943788</v>
       </c>
       <c r="U16" t="n">
-        <v>2.133330377330914</v>
+        <v>1.776943602557901</v>
       </c>
       <c r="V16" t="n">
-        <v>7.156860000193344</v>
+        <v>5.76135660508616</v>
       </c>
       <c r="W16" t="n">
-        <v>1.162420454577268</v>
+        <v>1.210024176498728</v>
       </c>
       <c r="X16" t="n">
-        <v>2.696142728797306</v>
+        <v>3.704147177524069</v>
       </c>
       <c r="Y16" t="n">
-        <v>1.589573025324983</v>
+        <v>1.369802357028365</v>
       </c>
       <c r="Z16" t="n">
-        <v>15.68856508732643</v>
+        <v>12.93781542431235</v>
       </c>
       <c r="AA16" t="n">
-        <v>1.068080169441658</v>
+        <v>1.083767420123067</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>6.712146686354352</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>1.175065532261082</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>33.07666439252557</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>1.031175311365387</v>
       </c>
     </row>
     <row r="17">
@@ -1957,73 +2157,85 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>4.863428848415707</v>
+        <v>4.425628848499814</v>
       </c>
       <c r="F17" t="n">
-        <v>9.432643862074315</v>
+        <v>9.038913286717641</v>
       </c>
       <c r="G17" t="n">
-        <v>1.452709367747507</v>
+        <v>1.507362011038076</v>
       </c>
       <c r="H17" t="n">
-        <v>8.025893590010636</v>
+        <v>7.169843991175479</v>
       </c>
       <c r="I17" t="n">
-        <v>2.295315058582717</v>
+        <v>2.159121284735777</v>
       </c>
       <c r="J17" t="n">
-        <v>1.772012950342878</v>
+        <v>1.862722489155181</v>
       </c>
       <c r="K17" t="n">
-        <v>1.142330649786925</v>
+        <v>1.162078652463542</v>
       </c>
       <c r="L17" t="n">
-        <v>14.45376339748106</v>
+        <v>12.66390675315545</v>
       </c>
       <c r="M17" t="n">
-        <v>1.768201987509289</v>
+        <v>1.687089492900077</v>
       </c>
       <c r="N17" t="n">
-        <v>2.301740969510194</v>
+        <v>2.455414484333308</v>
       </c>
       <c r="O17" t="n">
-        <v>1.074328644740938</v>
+        <v>1.085734567427802</v>
       </c>
       <c r="P17" t="n">
-        <v>2.967492086588453</v>
+        <v>24.40002825144752</v>
       </c>
       <c r="Q17" t="n">
-        <v>1.508261256457685</v>
+        <v>1.404943771477477</v>
       </c>
       <c r="R17" t="n">
-        <v>1.438502997677865</v>
+        <v>3.469478654657168</v>
       </c>
       <c r="S17" t="n">
-        <v>3.280486120495407</v>
+        <v>1.042734991139942</v>
       </c>
       <c r="T17" t="n">
-        <v>5.315603636355979</v>
+        <v>2.818444823029776</v>
       </c>
       <c r="U17" t="n">
-        <v>1.231717294789468</v>
+        <v>1.549920452540245</v>
       </c>
       <c r="V17" t="n">
-        <v>1.883678060871965</v>
+        <v>1.476352489521448</v>
       </c>
       <c r="W17" t="n">
-        <v>2.131633843000759</v>
+        <v>3.099285764213422</v>
       </c>
       <c r="X17" t="n">
-        <v>10.72596198137556</v>
+        <v>4.952441321501208</v>
       </c>
       <c r="Y17" t="n">
-        <v>1.102817592945039</v>
+        <v>1.253008183716737</v>
       </c>
       <c r="Z17" t="n">
-        <v>2.698792556125534</v>
+        <v>1.959910070178522</v>
       </c>
       <c r="AA17" t="n">
-        <v>1.588653391724719</v>
+        <v>2.041764255909955</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>9.791312240429161</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>1.113748661479823</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>2.852262880225011</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>1.539880170723132</v>
       </c>
     </row>
     <row r="18">
@@ -2048,73 +2260,85 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>1.126084766013845</v>
+        <v>1.1764419695738</v>
       </c>
       <c r="F18" t="n">
-        <v>19.47645016008061</v>
+        <v>15.49708051096329</v>
       </c>
       <c r="G18" t="n">
-        <v>16.49530087642855</v>
+        <v>11.70260780955664</v>
       </c>
       <c r="H18" t="n">
-        <v>1.231755168206504</v>
+        <v>1.316190028812062</v>
       </c>
       <c r="I18" t="n">
-        <v>1.030708859968578</v>
+        <v>1.046361835549002</v>
       </c>
       <c r="J18" t="n">
-        <v>33.56389201758787</v>
+        <v>22.56946523273572</v>
       </c>
       <c r="K18" t="n">
-        <v>5.314898380643479</v>
+        <v>4.162655077255404</v>
       </c>
       <c r="L18" t="n">
-        <v>1.40637707686559</v>
+        <v>1.545362514177303</v>
       </c>
       <c r="M18" t="n">
-        <v>1.013465105373599</v>
+        <v>1.021338126805855</v>
       </c>
       <c r="N18" t="n">
-        <v>75.26603596884593</v>
+        <v>47.86446983366951</v>
       </c>
       <c r="O18" t="n">
-        <v>3.460768721781897</v>
+        <v>2.833642712881602</v>
       </c>
       <c r="P18" t="n">
-        <v>1.181821200313999</v>
+        <v>1.918563979026671</v>
       </c>
       <c r="Q18" t="n">
-        <v>6.499908692017384</v>
+        <v>1.009048230098039</v>
       </c>
       <c r="R18" t="n">
-        <v>5.821808343592875</v>
+        <v>111.5188516610293</v>
       </c>
       <c r="S18" t="n">
-        <v>1.207391071718722</v>
+        <v>2.088655796256697</v>
       </c>
       <c r="T18" t="n">
-        <v>1.376449616587409</v>
+        <v>1.229357875951071</v>
       </c>
       <c r="U18" t="n">
-        <v>3.656397977145521</v>
+        <v>5.359998521321031</v>
       </c>
       <c r="V18" t="n">
-        <v>13.11688077431635</v>
+        <v>4.849271366489655</v>
       </c>
       <c r="W18" t="n">
-        <v>1.082529490767926</v>
+        <v>1.25978942630692</v>
       </c>
       <c r="X18" t="n">
-        <v>1.716639618927951</v>
+        <v>1.469542784393753</v>
       </c>
       <c r="Y18" t="n">
-        <v>2.395401501100287</v>
+        <v>3.129731375365813</v>
       </c>
       <c r="Z18" t="n">
-        <v>33.64963891889236</v>
+        <v>10.30112948495734</v>
       </c>
       <c r="AA18" t="n">
-        <v>1.030628210084779</v>
+        <v>1.107513824166978</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>1.891882688007872</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>2.121223691687099</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>24.85881852925363</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>1.041913223774006</v>
       </c>
     </row>
     <row r="19">
@@ -2139,73 +2363,85 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1.152322664199341</v>
+        <v>1.399990542550285</v>
       </c>
       <c r="F19" t="n">
-        <v>17.34202184683024</v>
+        <v>8.796859221647132</v>
       </c>
       <c r="G19" t="n">
-        <v>13.41847676669771</v>
+        <v>5.812854292369102</v>
       </c>
       <c r="H19" t="n">
-        <v>1.272992257148443</v>
+        <v>1.740128953774035</v>
       </c>
       <c r="I19" t="n">
-        <v>1.039859679483453</v>
+        <v>1.101733891642287</v>
       </c>
       <c r="J19" t="n">
-        <v>26.08800905976009</v>
+        <v>10.82956597705076</v>
       </c>
       <c r="K19" t="n">
-        <v>4.663107556403102</v>
+        <v>2.351115903385268</v>
       </c>
       <c r="L19" t="n">
-        <v>1.469748855046506</v>
+        <v>2.343597091044774</v>
       </c>
       <c r="M19" t="n">
-        <v>1.018304594619495</v>
+        <v>1.046168141501393</v>
       </c>
       <c r="N19" t="n">
-        <v>55.6310923998809</v>
+        <v>22.65995787311086</v>
       </c>
       <c r="O19" t="n">
-        <v>3.128797099252106</v>
+        <v>1.744270739096647</v>
       </c>
       <c r="P19" t="n">
-        <v>1.181972407588059</v>
+        <v>3.441429288583933</v>
       </c>
       <c r="Q19" t="n">
-        <v>6.495338624434505</v>
+        <v>1.019179872950635</v>
       </c>
       <c r="R19" t="n">
-        <v>4.648473522524207</v>
+        <v>53.13798874339766</v>
       </c>
       <c r="S19" t="n">
-        <v>1.274087229584209</v>
+        <v>1.409596134803484</v>
       </c>
       <c r="T19" t="n">
-        <v>1.376745797829693</v>
+        <v>1.923389692655602</v>
       </c>
       <c r="U19" t="n">
-        <v>3.654309632013595</v>
+        <v>2.08296638781409</v>
       </c>
       <c r="V19" t="n">
-        <v>9.738051921748589</v>
+        <v>7.079511263003193</v>
       </c>
       <c r="W19" t="n">
-        <v>1.114441984203716</v>
+        <v>1.164486906387606</v>
       </c>
       <c r="X19" t="n">
-        <v>1.717193977308257</v>
+        <v>2.895790733637381</v>
       </c>
       <c r="Y19" t="n">
-        <v>2.394322919098065</v>
+        <v>1.527484380135849</v>
       </c>
       <c r="Z19" t="n">
-        <v>23.16163723632053</v>
+        <v>16.95204170770465</v>
       </c>
       <c r="AA19" t="n">
-        <v>1.045123019988844</v>
+        <v>1.062687900290344</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>4.848014056285145</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>1.259874310585392</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>46.31575200177343</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>1.022067381778435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Versão com 3n, com teams goals adicionado e future_match com 0x0
</commit_message>
<xml_diff>
--- a/output_corners_NNNN_AH.xlsx
+++ b/output_corners_NNNN_AH.xlsx
@@ -612,85 +612,85 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2.312791972610813</v>
+        <v>1.923336850859044</v>
       </c>
       <c r="F2" t="n">
-        <v>6.785086207772856</v>
+        <v>6.93617069790043</v>
       </c>
       <c r="G2" t="n">
-        <v>2.379592068190155</v>
+        <v>2.977089752965037</v>
       </c>
       <c r="H2" t="n">
-        <v>3.397825518057425</v>
+        <v>2.676455202283481</v>
       </c>
       <c r="I2" t="n">
-        <v>1.396083645024922</v>
+        <v>1.270351708665753</v>
       </c>
       <c r="J2" t="n">
-        <v>3.524719241909316</v>
+        <v>4.698885444206093</v>
       </c>
       <c r="K2" t="n">
-        <v>1.417044523243768</v>
+        <v>1.596496702469539</v>
       </c>
       <c r="L2" t="n">
-        <v>5.499148675577953</v>
+        <v>4.085488626355449</v>
       </c>
       <c r="M2" t="n">
-        <v>1.210286789279645</v>
+        <v>1.13845035605351</v>
       </c>
       <c r="N2" t="n">
-        <v>5.755410472648263</v>
+        <v>8.222805549257739</v>
       </c>
       <c r="O2" t="n">
-        <v>1.222264270889324</v>
+        <v>1.324097775457105</v>
       </c>
       <c r="P2" t="n">
-        <v>9.821679661730025</v>
+        <v>6.860976526401542</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.106648910267894</v>
+        <v>1.066841892581375</v>
       </c>
       <c r="R2" t="n">
-        <v>10.37656088081988</v>
+        <v>15.96067752394323</v>
       </c>
       <c r="S2" t="n">
-        <v>1.113357097326734</v>
+        <v>1.170620031575859</v>
       </c>
       <c r="T2" t="n">
-        <v>2.982042807462987</v>
+        <v>2.571316121629716</v>
       </c>
       <c r="U2" t="n">
-        <v>1.5045299709142</v>
+        <v>1.636409177144338</v>
       </c>
       <c r="V2" t="n">
-        <v>3.057572513042207</v>
+        <v>3.793967815533039</v>
       </c>
       <c r="W2" t="n">
-        <v>1.486009602899223</v>
+        <v>1.357913929588061</v>
       </c>
       <c r="X2" t="n">
-        <v>5.351343948514389</v>
+        <v>4.362525098916177</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.229814055572742</v>
+        <v>1.297395549648781</v>
       </c>
       <c r="Z2" t="n">
-        <v>5.537666914872359</v>
+        <v>7.420305257246379</v>
       </c>
       <c r="AA2" t="n">
-        <v>1.220377568199743</v>
+        <v>1.155755834019159</v>
       </c>
       <c r="AB2" t="n">
-        <v>10.81880282873611</v>
+        <v>8.308868274860352</v>
       </c>
       <c r="AC2" t="n">
-        <v>1.101845410020187</v>
+        <v>1.136820087925187</v>
       </c>
       <c r="AD2" t="n">
-        <v>11.30521869351856</v>
+        <v>16.42592156678145</v>
       </c>
       <c r="AE2" t="n">
-        <v>1.097038212360204</v>
+        <v>1.064825948691028</v>
       </c>
     </row>
     <row r="3">
@@ -715,85 +715,85 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1.175568535820792</v>
+        <v>1.183924986501544</v>
       </c>
       <c r="F3" t="n">
-        <v>15.54541914979087</v>
+        <v>15.16733065196016</v>
       </c>
       <c r="G3" t="n">
-        <v>11.76191966543118</v>
+        <v>11.1830914060697</v>
       </c>
       <c r="H3" t="n">
-        <v>1.31475633059442</v>
+        <v>1.327492805707095</v>
       </c>
       <c r="I3" t="n">
-        <v>1.04607386981364</v>
+        <v>1.049224832354532</v>
       </c>
       <c r="J3" t="n">
-        <v>22.70427628599033</v>
+        <v>21.31494983665363</v>
       </c>
       <c r="K3" t="n">
-        <v>4.177060801641351</v>
+        <v>4.053502191722607</v>
       </c>
       <c r="L3" t="n">
-        <v>1.543038721401227</v>
+        <v>1.56213076545669</v>
       </c>
       <c r="M3" t="n">
-        <v>1.021188018408338</v>
+        <v>1.022931349288499</v>
       </c>
       <c r="N3" t="n">
-        <v>48.19648533090184</v>
+        <v>44.60842388378578</v>
       </c>
       <c r="O3" t="n">
-        <v>2.841489309306812</v>
+        <v>2.778945507790476</v>
       </c>
       <c r="P3" t="n">
-        <v>1.914776842152114</v>
+        <v>1.943455431974953</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.008976212066859</v>
+        <v>1.009859504391711</v>
       </c>
       <c r="R3" t="n">
-        <v>112.4055675770049</v>
+        <v>102.4249763751488</v>
       </c>
       <c r="S3" t="n">
-        <v>2.093162784540313</v>
+        <v>2.059933480807547</v>
       </c>
       <c r="T3" t="n">
-        <v>1.22875781535031</v>
+        <v>1.226177208500193</v>
       </c>
       <c r="U3" t="n">
-        <v>5.371435347328531</v>
+        <v>5.421311973169682</v>
       </c>
       <c r="V3" t="n">
-        <v>4.866051527315383</v>
+        <v>4.557419825046391</v>
       </c>
       <c r="W3" t="n">
-        <v>1.258661839588674</v>
+        <v>1.281102610650392</v>
       </c>
       <c r="X3" t="n">
-        <v>1.468367131900277</v>
+        <v>1.463311489636002</v>
       </c>
       <c r="Y3" t="n">
-        <v>3.13507723298764</v>
+        <v>3.158375137179619</v>
       </c>
       <c r="Z3" t="n">
-        <v>10.34848236615096</v>
+        <v>9.484925860336233</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.106969234238576</v>
+        <v>1.117856068097733</v>
       </c>
       <c r="AB3" t="n">
-        <v>1.889656460753628</v>
+        <v>1.880087004003894</v>
       </c>
       <c r="AC3" t="n">
-        <v>2.124029380006863</v>
+        <v>2.13625129725876</v>
       </c>
       <c r="AD3" t="n">
-        <v>25.00253622135297</v>
+        <v>22.40594182878175</v>
       </c>
       <c r="AE3" t="n">
-        <v>1.041662263969855</v>
+        <v>1.046716001005638</v>
       </c>
     </row>
     <row r="4">
@@ -818,85 +818,85 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>4.008872943892104</v>
+        <v>1.976052193185719</v>
       </c>
       <c r="F4" t="n">
-        <v>8.763026311373036</v>
+        <v>6.928795560379236</v>
       </c>
       <c r="G4" t="n">
-        <v>1.571246184884417</v>
+        <v>2.860287013789794</v>
       </c>
       <c r="H4" t="n">
-        <v>6.336422106173567</v>
+        <v>2.766723018385874</v>
       </c>
       <c r="I4" t="n">
-        <v>2.03688767920148</v>
+        <v>1.289631961782188</v>
       </c>
       <c r="J4" t="n">
-        <v>1.964424614216761</v>
+        <v>4.452657620542691</v>
       </c>
       <c r="K4" t="n">
-        <v>1.187391473182589</v>
+        <v>1.566019681406329</v>
       </c>
       <c r="L4" t="n">
-        <v>10.89053649828339</v>
+        <v>4.247891085442803</v>
       </c>
       <c r="M4" t="n">
-        <v>1.616838986886146</v>
+        <v>1.14993940642893</v>
       </c>
       <c r="N4" t="n">
-        <v>2.621168605194822</v>
+        <v>7.669360802585214</v>
       </c>
       <c r="O4" t="n">
-        <v>1.101106749889004</v>
+        <v>1.307892097885316</v>
       </c>
       <c r="P4" t="n">
-        <v>20.37033672575985</v>
+        <v>7.171894160685237</v>
       </c>
       <c r="Q4" t="n">
-        <v>1.363694527315796</v>
+        <v>1.073388008538861</v>
       </c>
       <c r="R4" t="n">
-        <v>3.749560207519155</v>
+        <v>14.62620433378397</v>
       </c>
       <c r="S4" t="n">
-        <v>1.05162532867434</v>
+        <v>1.162024813447057</v>
       </c>
       <c r="T4" t="n">
-        <v>2.564516363900642</v>
+        <v>2.573923406736804</v>
       </c>
       <c r="U4" t="n">
-        <v>1.639175161777667</v>
+        <v>1.635354932596935</v>
       </c>
       <c r="V4" t="n">
-        <v>1.488167319172882</v>
+        <v>3.556576773089214</v>
       </c>
       <c r="W4" t="n">
-        <v>3.048477972049281</v>
+        <v>1.391148042384684</v>
       </c>
       <c r="X4" t="n">
-        <v>4.346517151790643</v>
+        <v>4.36866640204015</v>
       </c>
       <c r="Y4" t="n">
-        <v>1.29881813080352</v>
+        <v>1.296853377762302</v>
       </c>
       <c r="Z4" t="n">
-        <v>1.983798907094109</v>
+        <v>6.800892868441699</v>
       </c>
       <c r="AA4" t="n">
-        <v>2.016467890733631</v>
+        <v>1.172387255320685</v>
       </c>
       <c r="AB4" t="n">
-        <v>8.269294338018137</v>
+        <v>8.324059955774208</v>
       </c>
       <c r="AC4" t="n">
-        <v>1.137564934572815</v>
+        <v>1.13653629353643</v>
       </c>
       <c r="AD4" t="n">
-        <v>2.90066270798861</v>
+        <v>14.70242916771907</v>
       </c>
       <c r="AE4" t="n">
-        <v>1.526132277861261</v>
+        <v>1.072979760578209</v>
       </c>
     </row>
     <row r="5">
@@ -921,85 +921,85 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1.17657081177442</v>
+        <v>1.183952510714555</v>
       </c>
       <c r="F5" t="n">
-        <v>15.49871908696802</v>
+        <v>15.16608951030253</v>
       </c>
       <c r="G5" t="n">
-        <v>11.68894169891993</v>
+        <v>11.18131074225491</v>
       </c>
       <c r="H5" t="n">
-        <v>1.316279221522278</v>
+        <v>1.327535440297096</v>
       </c>
       <c r="I5" t="n">
-        <v>1.046452213283515</v>
+        <v>1.049234982198739</v>
       </c>
       <c r="J5" t="n">
-        <v>22.52749953800097</v>
+        <v>21.31076188803062</v>
       </c>
       <c r="K5" t="n">
-        <v>4.161763188827003</v>
+        <v>4.053104723851984</v>
       </c>
       <c r="L5" t="n">
-        <v>1.545311076095041</v>
+        <v>1.562195919670987</v>
       </c>
       <c r="M5" t="n">
-        <v>1.021396912952841</v>
+        <v>1.022936930246082</v>
       </c>
       <c r="N5" t="n">
-        <v>47.73571380151992</v>
+        <v>44.59781318909644</v>
       </c>
       <c r="O5" t="n">
-        <v>2.83381567666106</v>
+        <v>2.778739341589723</v>
       </c>
       <c r="P5" t="n">
-        <v>1.918170088370768</v>
+        <v>1.943555494920996</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.009081668529155</v>
+        <v>1.009862322920857</v>
       </c>
       <c r="R5" t="n">
-        <v>111.1119245642625</v>
+        <v>102.3959903792231</v>
       </c>
       <c r="S5" t="n">
-        <v>2.089122824480628</v>
+        <v>2.059821076113526</v>
       </c>
       <c r="T5" t="n">
-        <v>1.228380907572516</v>
+        <v>1.226175279764877</v>
       </c>
       <c r="U5" t="n">
-        <v>5.378649733154581</v>
+        <v>5.421349676408319</v>
       </c>
       <c r="V5" t="n">
-        <v>4.825515409606563</v>
+        <v>4.556589152792879</v>
       </c>
       <c r="W5" t="n">
-        <v>1.261402685109781</v>
+        <v>1.281168264603948</v>
       </c>
       <c r="X5" t="n">
-        <v>1.467628701235015</v>
+        <v>1.463307711269392</v>
       </c>
       <c r="Y5" t="n">
-        <v>3.138448725150922</v>
+        <v>3.158392739158502</v>
       </c>
       <c r="Z5" t="n">
-        <v>10.23416901756683</v>
+        <v>9.482623066596688</v>
       </c>
       <c r="AA5" t="n">
-        <v>1.108293447747992</v>
+        <v>1.117888062707614</v>
       </c>
       <c r="AB5" t="n">
-        <v>1.888258338901582</v>
+        <v>1.8800798546061</v>
       </c>
       <c r="AC5" t="n">
-        <v>2.125798606334051</v>
+        <v>2.13626052768538</v>
       </c>
       <c r="AD5" t="n">
-        <v>24.65584981744083</v>
+        <v>22.39908810299136</v>
       </c>
       <c r="AE5" t="n">
-        <v>1.042272841927781</v>
+        <v>1.046730963262879</v>
       </c>
     </row>
     <row r="6">
@@ -1024,85 +1024,85 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1.175553945631493</v>
+        <v>1.184017270993913</v>
       </c>
       <c r="F6" t="n">
-        <v>15.54966981035253</v>
+        <v>15.16300977774388</v>
       </c>
       <c r="G6" t="n">
-        <v>11.76094762692905</v>
+        <v>11.17721090695554</v>
       </c>
       <c r="H6" t="n">
-        <v>1.31468454835281</v>
+        <v>1.327638102363453</v>
       </c>
       <c r="I6" t="n">
-        <v>1.046087756948969</v>
+        <v>1.049257927277037</v>
       </c>
       <c r="J6" t="n">
-        <v>22.69773636645521</v>
+        <v>21.30130083175839</v>
       </c>
       <c r="K6" t="n">
-        <v>4.177785516430398</v>
+        <v>4.052148064545579</v>
       </c>
       <c r="L6" t="n">
-        <v>1.542845682779898</v>
+        <v>1.562356776524866</v>
       </c>
       <c r="M6" t="n">
-        <v>1.021199797788762</v>
+        <v>1.022949337935481</v>
       </c>
       <c r="N6" t="n">
-        <v>48.17026124325213</v>
+        <v>44.57424178472493</v>
       </c>
       <c r="O6" t="n">
-        <v>2.842144152052618</v>
+        <v>2.778230549971477</v>
       </c>
       <c r="P6" t="n">
-        <v>1.914340945799745</v>
+        <v>1.943809177353353</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.008983892002674</v>
+        <v>1.009868498370555</v>
       </c>
       <c r="R6" t="n">
-        <v>112.3103318363967</v>
+        <v>102.3325394047489</v>
       </c>
       <c r="S6" t="n">
-        <v>2.093683931135045</v>
+        <v>2.059536211339053</v>
       </c>
       <c r="T6" t="n">
-        <v>1.228330056759684</v>
+        <v>1.226190641231091</v>
       </c>
       <c r="U6" t="n">
-        <v>5.379624891227056</v>
+        <v>5.42104940574591</v>
       </c>
       <c r="V6" t="n">
-        <v>4.857904622083269</v>
+        <v>4.55500347446733</v>
       </c>
       <c r="W6" t="n">
-        <v>1.259208067062062</v>
+        <v>1.281293677258596</v>
       </c>
       <c r="X6" t="n">
-        <v>1.467529076191523</v>
+        <v>1.463337804183686</v>
       </c>
       <c r="Y6" t="n">
-        <v>3.138904403862898</v>
+        <v>3.158252555631222</v>
       </c>
       <c r="Z6" t="n">
-        <v>10.32548648264921</v>
+        <v>9.478227566628307</v>
       </c>
       <c r="AA6" t="n">
-        <v>1.107233011581817</v>
+        <v>1.117949181257668</v>
       </c>
       <c r="AB6" t="n">
-        <v>1.888069722412551</v>
+        <v>1.880136796298589</v>
       </c>
       <c r="AC6" t="n">
-        <v>2.126037713889599</v>
+        <v>2.13618701570653</v>
       </c>
       <c r="AD6" t="n">
-        <v>24.93272400712383</v>
+        <v>22.38600699454496</v>
       </c>
       <c r="AE6" t="n">
-        <v>1.041783793591667</v>
+        <v>1.046759547037232</v>
       </c>
     </row>
     <row r="7">
@@ -1127,85 +1127,85 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1.571744492928856</v>
+        <v>1.351394271588273</v>
       </c>
       <c r="F7" t="n">
-        <v>7.478886211391416</v>
+        <v>9.460477217228302</v>
       </c>
       <c r="G7" t="n">
-        <v>4.346795635137402</v>
+        <v>6.480016722913374</v>
       </c>
       <c r="H7" t="n">
-        <v>2.064916339067152</v>
+        <v>1.648034471860553</v>
       </c>
       <c r="I7" t="n">
-        <v>1.148811678389527</v>
+        <v>1.089073986103413</v>
       </c>
       <c r="J7" t="n">
-        <v>7.719902704023132</v>
+        <v>12.22662231416283</v>
       </c>
       <c r="K7" t="n">
-        <v>1.939040902382981</v>
+        <v>2.543127786287245</v>
       </c>
       <c r="L7" t="n">
-        <v>2.972962167471333</v>
+        <v>2.167402863746525</v>
       </c>
       <c r="M7" t="n">
-        <v>1.069299347074809</v>
+        <v>1.040225757101051</v>
       </c>
       <c r="N7" t="n">
-        <v>15.43015038684983</v>
+        <v>25.85969369048545</v>
       </c>
       <c r="O7" t="n">
-        <v>1.506852090976311</v>
+        <v>1.856602318749431</v>
       </c>
       <c r="P7" t="n">
-        <v>4.712562281198177</v>
+        <v>3.094710232833723</v>
       </c>
       <c r="Q7" t="n">
-        <v>1.029723651130022</v>
+        <v>1.016616080590049</v>
       </c>
       <c r="R7" t="n">
-        <v>34.64324240066055</v>
+        <v>61.18266429201447</v>
       </c>
       <c r="S7" t="n">
-        <v>1.269355750626563</v>
+        <v>1.477392998957761</v>
       </c>
       <c r="T7" t="n">
-        <v>2.395777500845176</v>
+        <v>1.775149402986787</v>
       </c>
       <c r="U7" t="n">
-        <v>1.716446567876668</v>
+        <v>2.290073882720963</v>
       </c>
       <c r="V7" t="n">
-        <v>6.545201489579058</v>
+        <v>7.027394550635948</v>
       </c>
       <c r="W7" t="n">
-        <v>1.180336098134445</v>
+        <v>1.16590916549415</v>
       </c>
       <c r="X7" t="n">
-        <v>3.953263510630933</v>
+        <v>2.578157813736328</v>
       </c>
       <c r="Y7" t="n">
-        <v>1.338608456847916</v>
+        <v>1.633650190935262</v>
       </c>
       <c r="Z7" t="n">
-        <v>15.29802753557291</v>
+        <v>16.78917916015097</v>
       </c>
       <c r="AA7" t="n">
-        <v>1.069939717035237</v>
+        <v>1.063334514724098</v>
       </c>
       <c r="AB7" t="n">
-        <v>7.308667115700426</v>
+        <v>4.149051493512012</v>
       </c>
       <c r="AC7" t="n">
-        <v>1.158512088474488</v>
+        <v>1.317555937735632</v>
       </c>
       <c r="AD7" t="n">
-        <v>40.76492614841345</v>
+        <v>45.76363851907432</v>
       </c>
       <c r="AE7" t="n">
-        <v>1.02514778969456</v>
+        <v>1.022339560256566</v>
       </c>
     </row>
     <row r="8">
@@ -1230,85 +1230,85 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1.510373371217801</v>
+        <v>1.904937168886584</v>
       </c>
       <c r="F8" t="n">
-        <v>8.414874654394533</v>
+        <v>6.968211779276791</v>
       </c>
       <c r="G8" t="n">
-        <v>4.564649458239582</v>
+        <v>3.016232204726836</v>
       </c>
       <c r="H8" t="n">
-        <v>1.904803896753523</v>
+        <v>2.640932447435846</v>
       </c>
       <c r="I8" t="n">
-        <v>1.147745297522529</v>
+        <v>1.265061382637402</v>
       </c>
       <c r="J8" t="n">
-        <v>7.768404929080861</v>
+        <v>4.772711022819869</v>
       </c>
       <c r="K8" t="n">
-        <v>2.105211862579334</v>
+        <v>1.609409608276453</v>
       </c>
       <c r="L8" t="n">
-        <v>2.590248612781015</v>
+        <v>4.01371843658422</v>
       </c>
       <c r="M8" t="n">
-        <v>1.073415589581014</v>
+        <v>1.13564087320727</v>
       </c>
       <c r="N8" t="n">
-        <v>14.62108519058491</v>
+        <v>8.372409041277084</v>
       </c>
       <c r="O8" t="n">
-        <v>1.628832493210737</v>
+        <v>1.331816001077198</v>
       </c>
       <c r="P8" t="n">
-        <v>3.817761085606752</v>
+        <v>6.70757121517873</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.033987009466157</v>
+        <v>1.065407094502636</v>
       </c>
       <c r="R8" t="n">
-        <v>30.42300648710465</v>
+        <v>16.28886136288612</v>
       </c>
       <c r="S8" t="n">
-        <v>1.354891692240355</v>
+        <v>1.175205873444136</v>
       </c>
       <c r="T8" t="n">
-        <v>1.773654591072937</v>
+        <v>2.532379755221637</v>
       </c>
       <c r="U8" t="n">
-        <v>2.292566490962275</v>
+        <v>1.652579751587337</v>
       </c>
       <c r="V8" t="n">
-        <v>4.176233839933125</v>
+        <v>3.805289316703965</v>
       </c>
       <c r="W8" t="n">
-        <v>1.314838280301508</v>
+        <v>1.356469471453638</v>
       </c>
       <c r="X8" t="n">
-        <v>2.574991314343375</v>
+        <v>4.271027741815391</v>
       </c>
       <c r="Y8" t="n">
-        <v>1.634924136338433</v>
+        <v>1.305714313338415</v>
       </c>
       <c r="Z8" t="n">
-        <v>8.440795556009052</v>
+        <v>7.450127065688388</v>
       </c>
       <c r="AA8" t="n">
-        <v>1.134394231433011</v>
+        <v>1.155035705469978</v>
       </c>
       <c r="AB8" t="n">
-        <v>4.142188664816253</v>
+        <v>8.083159160037358</v>
       </c>
       <c r="AC8" t="n">
-        <v>1.318249509075381</v>
+        <v>1.141179942086001</v>
       </c>
       <c r="AD8" t="n">
-        <v>19.33903563101921</v>
+        <v>16.50978338716183</v>
       </c>
       <c r="AE8" t="n">
-        <v>1.054528494306896</v>
+        <v>1.064475433024277</v>
       </c>
     </row>
     <row r="9">
@@ -1333,85 +1333,85 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1.175520022706314</v>
+        <v>1.184383151524549</v>
       </c>
       <c r="F9" t="n">
-        <v>15.55231180122081</v>
+        <v>15.14377111265257</v>
       </c>
       <c r="G9" t="n">
-        <v>11.76283231838263</v>
+        <v>11.15512626180548</v>
       </c>
       <c r="H9" t="n">
-        <v>1.314618381719359</v>
+        <v>1.328245595125627</v>
       </c>
       <c r="I9" t="n">
-        <v>1.046080674037752</v>
+        <v>1.049376620092058</v>
       </c>
       <c r="J9" t="n">
-        <v>22.70107145526457</v>
+        <v>21.25250003211253</v>
       </c>
       <c r="K9" t="n">
-        <v>4.178453828842092</v>
+        <v>4.046499373791377</v>
       </c>
       <c r="L9" t="n">
-        <v>1.542721638142272</v>
+        <v>1.563354001779139</v>
       </c>
       <c r="M9" t="n">
-        <v>1.021197102404618</v>
+        <v>1.023010981369475</v>
       </c>
       <c r="N9" t="n">
-        <v>48.17625932599739</v>
+        <v>44.45751204364343</v>
       </c>
       <c r="O9" t="n">
-        <v>2.842565193131022</v>
+        <v>2.775082802007052</v>
       </c>
       <c r="P9" t="n">
-        <v>1.914112233923191</v>
+        <v>1.945455953942015</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.00898304438841</v>
+        <v>1.009898056015272</v>
       </c>
       <c r="R9" t="n">
-        <v>112.3208347595676</v>
+        <v>102.0299394605406</v>
       </c>
       <c r="S9" t="n">
-        <v>2.093957572045827</v>
+        <v>2.057690732001388</v>
       </c>
       <c r="T9" t="n">
-        <v>1.228215250349452</v>
+        <v>1.226510098524577</v>
       </c>
       <c r="U9" t="n">
-        <v>5.381828113891434</v>
+        <v>5.414814202606054</v>
       </c>
       <c r="V9" t="n">
-        <v>4.856711931340955</v>
+        <v>4.550354074691479</v>
       </c>
       <c r="W9" t="n">
-        <v>1.259288227330037</v>
+        <v>1.281662048055559</v>
       </c>
       <c r="X9" t="n">
-        <v>1.467304152489848</v>
+        <v>1.463963621097726</v>
       </c>
       <c r="Y9" t="n">
-        <v>3.139933905298917</v>
+        <v>3.15534139860799</v>
       </c>
       <c r="Z9" t="n">
-        <v>10.3221208290261</v>
+        <v>9.465341894060328</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.107271726932172</v>
+        <v>1.118128719727392</v>
       </c>
       <c r="AB9" t="n">
-        <v>1.887643891683332</v>
+        <v>1.881321015968066</v>
       </c>
       <c r="AC9" t="n">
-        <v>2.126577909643016</v>
+        <v>2.134660335884053</v>
       </c>
       <c r="AD9" t="n">
-        <v>24.92250935344757</v>
+        <v>22.34766701219579</v>
       </c>
       <c r="AE9" t="n">
-        <v>1.041801634821218</v>
+        <v>1.046843526247093</v>
       </c>
     </row>
     <row r="10">
@@ -1436,85 +1436,85 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>4.263535613010567</v>
+        <v>4.586898710139524</v>
       </c>
       <c r="F10" t="n">
-        <v>8.892132260944718</v>
+        <v>9.349774840402226</v>
       </c>
       <c r="G10" t="n">
-        <v>1.531407841590183</v>
+        <v>1.481408340814993</v>
       </c>
       <c r="H10" t="n">
-        <v>6.857260346271354</v>
+        <v>7.419198195676522</v>
       </c>
       <c r="I10" t="n">
-        <v>2.10754727172351</v>
+        <v>2.230491039320907</v>
       </c>
       <c r="J10" t="n">
-        <v>1.902895998690738</v>
+        <v>1.812683691343164</v>
       </c>
       <c r="K10" t="n">
-        <v>1.170728282658049</v>
+        <v>1.155782695831626</v>
       </c>
       <c r="L10" t="n">
-        <v>12.02012188810848</v>
+        <v>13.05249047613408</v>
       </c>
       <c r="M10" t="n">
-        <v>1.656133303482119</v>
+        <v>1.735678925487833</v>
       </c>
       <c r="N10" t="n">
-        <v>2.524080540787931</v>
+        <v>2.359288631704238</v>
       </c>
       <c r="O10" t="n">
-        <v>1.090743097957843</v>
+        <v>1.082970403667206</v>
       </c>
       <c r="P10" t="n">
-        <v>22.97834288521315</v>
+        <v>24.9913311395622</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.385947942075676</v>
+        <v>1.438143427525581</v>
       </c>
       <c r="R10" t="n">
-        <v>3.591023013678673</v>
+        <v>3.282357641760165</v>
       </c>
       <c r="S10" t="n">
-        <v>1.045499335651588</v>
+        <v>1.041681722209693</v>
       </c>
       <c r="T10" t="n">
-        <v>2.765509237841624</v>
+        <v>2.672832229631065</v>
       </c>
       <c r="U10" t="n">
-        <v>1.566408817674907</v>
+        <v>1.597788578129287</v>
       </c>
       <c r="V10" t="n">
-        <v>1.493782555300931</v>
+        <v>1.411591504717847</v>
       </c>
       <c r="W10" t="n">
-        <v>3.025182925691979</v>
+        <v>3.429593391840088</v>
       </c>
       <c r="X10" t="n">
-        <v>4.824772746352181</v>
+        <v>4.60295685513101</v>
       </c>
       <c r="Y10" t="n">
-        <v>1.261453442156461</v>
+        <v>1.277549812614572</v>
       </c>
       <c r="Z10" t="n">
-        <v>1.995168236546222</v>
+        <v>1.829745563653429</v>
       </c>
       <c r="AA10" t="n">
-        <v>2.00485522274158</v>
+        <v>2.205188727490061</v>
       </c>
       <c r="AB10" t="n">
-        <v>9.466621393855874</v>
+        <v>8.90749337734746</v>
       </c>
       <c r="AC10" t="n">
-        <v>1.118110867780823</v>
+        <v>1.126462325326088</v>
       </c>
       <c r="AD10" t="n">
-        <v>2.923748394645408</v>
+        <v>2.591127467430399</v>
       </c>
       <c r="AE10" t="n">
-        <v>1.519818497462254</v>
+        <v>1.628485159403951</v>
       </c>
     </row>
     <row r="11">
@@ -1539,85 +1539,85 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1.178969611469527</v>
+        <v>1.184448199371951</v>
       </c>
       <c r="F11" t="n">
-        <v>15.3850369280119</v>
+        <v>15.14174163551137</v>
       </c>
       <c r="G11" t="n">
-        <v>11.52027305145817</v>
+        <v>11.15045958879614</v>
       </c>
       <c r="H11" t="n">
-        <v>1.319978156383952</v>
+        <v>1.328333330451867</v>
       </c>
       <c r="I11" t="n">
-        <v>1.047338049926346</v>
+        <v>1.049405811450337</v>
       </c>
       <c r="J11" t="n">
-        <v>22.1246555689536</v>
+        <v>21.24053386928397</v>
       </c>
       <c r="K11" t="n">
-        <v>4.12521333112523</v>
+        <v>4.045685305916873</v>
       </c>
       <c r="L11" t="n">
-        <v>1.550926604745412</v>
+        <v>1.563466105561978</v>
       </c>
       <c r="M11" t="n">
-        <v>1.021882359864325</v>
+        <v>1.023028199287424</v>
       </c>
       <c r="N11" t="n">
-        <v>46.69891027294187</v>
+        <v>44.42501936511045</v>
       </c>
       <c r="O11" t="n">
-        <v>2.815123813928189</v>
+        <v>2.77472964234937</v>
       </c>
       <c r="P11" t="n">
-        <v>1.92672343389757</v>
+        <v>1.945591374331092</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.009325396862301</v>
+        <v>1.009907260880814</v>
       </c>
       <c r="R11" t="n">
-        <v>108.2340421288221</v>
+        <v>101.9360722433978</v>
       </c>
       <c r="S11" t="n">
-        <v>2.079070587213109</v>
+        <v>2.057539257596757</v>
       </c>
       <c r="T11" t="n">
-        <v>1.227976925784149</v>
+        <v>1.226395470965047</v>
       </c>
       <c r="U11" t="n">
-        <v>5.3864088287023</v>
+        <v>5.417049491923759</v>
       </c>
       <c r="V11" t="n">
-        <v>4.740801488338272</v>
+        <v>4.546374888258343</v>
       </c>
       <c r="W11" t="n">
-        <v>1.267322391502848</v>
+        <v>1.281978085089337</v>
       </c>
       <c r="X11" t="n">
-        <v>1.46683724093097</v>
+        <v>1.463739064758288</v>
       </c>
       <c r="Y11" t="n">
-        <v>3.142074179870039</v>
+        <v>3.156385079443815</v>
       </c>
       <c r="Z11" t="n">
-        <v>9.996135120450173</v>
+        <v>9.45431661616168</v>
       </c>
       <c r="AA11" t="n">
-        <v>1.111158846172373</v>
+        <v>1.118282771441083</v>
       </c>
       <c r="AB11" t="n">
-        <v>1.886759964560253</v>
+        <v>1.880896081630238</v>
       </c>
       <c r="AC11" t="n">
-        <v>2.127700888589285</v>
+        <v>2.135207683236985</v>
       </c>
       <c r="AD11" t="n">
-        <v>23.93680582629139</v>
+        <v>22.31487200787445</v>
       </c>
       <c r="AE11" t="n">
-        <v>1.043598049683699</v>
+        <v>1.04691559956966</v>
       </c>
     </row>
     <row r="12">
@@ -1642,85 +1642,85 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>2.572616680830862</v>
+        <v>4.395973212565194</v>
       </c>
       <c r="F12" t="n">
-        <v>7.279034277707837</v>
+        <v>9.1802112366922</v>
       </c>
       <c r="G12" t="n">
-        <v>2.110105962872146</v>
+        <v>1.506956567420807</v>
       </c>
       <c r="H12" t="n">
-        <v>3.783863006151783</v>
+        <v>7.050177112164888</v>
       </c>
       <c r="I12" t="n">
-        <v>1.514952608621186</v>
+        <v>2.170193715924846</v>
       </c>
       <c r="J12" t="n">
-        <v>2.941926272939088</v>
+        <v>1.854559366018868</v>
       </c>
       <c r="K12" t="n">
-        <v>1.359213078298106</v>
+        <v>1.165284417540329</v>
       </c>
       <c r="L12" t="n">
-        <v>6.075165128199338</v>
+        <v>12.29206702878279</v>
       </c>
       <c r="M12" t="n">
-        <v>1.289191860407991</v>
+        <v>1.699610865239598</v>
       </c>
       <c r="N12" t="n">
-        <v>4.45791198476058</v>
+        <v>2.429366022864048</v>
       </c>
       <c r="O12" t="n">
-        <v>1.197037923838904</v>
+        <v>1.088557745667915</v>
       </c>
       <c r="P12" t="n">
-        <v>10.66632182911704</v>
+        <v>23.31458591067049</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.15718837056945</v>
+        <v>1.4160512139852</v>
       </c>
       <c r="R12" t="n">
-        <v>7.361793791597162</v>
+        <v>3.403550251473543</v>
       </c>
       <c r="S12" t="n">
-        <v>1.103451966288541</v>
+        <v>1.044813737705158</v>
       </c>
       <c r="T12" t="n">
-        <v>2.507062990172581</v>
+        <v>2.609077111600766</v>
       </c>
       <c r="U12" t="n">
-        <v>1.663542271637555</v>
+        <v>1.621474255516049</v>
       </c>
       <c r="V12" t="n">
-        <v>2.172168523422857</v>
+        <v>1.426033793345391</v>
       </c>
       <c r="W12" t="n">
-        <v>1.85311964962162</v>
+        <v>3.347231641292095</v>
       </c>
       <c r="X12" t="n">
-        <v>4.211752849620511</v>
+        <v>4.451643939598328</v>
       </c>
       <c r="Y12" t="n">
-        <v>1.31135646073083</v>
+        <v>1.289717021077316</v>
       </c>
       <c r="Z12" t="n">
-        <v>3.444414755749374</v>
+        <v>1.858661551069982</v>
       </c>
       <c r="AA12" t="n">
-        <v>1.40909587771386</v>
+        <v>2.16460321153765</v>
       </c>
       <c r="AB12" t="n">
-        <v>7.937571260544279</v>
+        <v>8.529833717140793</v>
       </c>
       <c r="AC12" t="n">
-        <v>1.14414266354095</v>
+        <v>1.132805057530502</v>
       </c>
       <c r="AD12" t="n">
-        <v>6.100786838470794</v>
+        <v>2.648757572936995</v>
       </c>
       <c r="AE12" t="n">
-        <v>1.196048184656114</v>
+        <v>1.606517305160068</v>
       </c>
     </row>
     <row r="13">
@@ -1745,85 +1745,85 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2.06457301509098</v>
+        <v>2.124730399453318</v>
       </c>
       <c r="F13" t="n">
-        <v>6.952995651537126</v>
+        <v>7.010724870846568</v>
       </c>
       <c r="G13" t="n">
-        <v>2.68950634220995</v>
+        <v>2.585894022788549</v>
       </c>
       <c r="H13" t="n">
-        <v>2.915418059260459</v>
+        <v>3.011125257968979</v>
       </c>
       <c r="I13" t="n">
-        <v>1.323270044131755</v>
+        <v>1.348206726927858</v>
       </c>
       <c r="J13" t="n">
-        <v>4.093389004495664</v>
+        <v>3.871857212015273</v>
       </c>
       <c r="K13" t="n">
-        <v>1.522079237566601</v>
+        <v>1.497234071342674</v>
       </c>
       <c r="L13" t="n">
-        <v>4.509964855237964</v>
+        <v>4.667970503819315</v>
       </c>
       <c r="M13" t="n">
-        <v>1.17042012987283</v>
+        <v>1.186195340499351</v>
       </c>
       <c r="N13" t="n">
-        <v>6.86785141371627</v>
+        <v>6.37070367775121</v>
       </c>
       <c r="O13" t="n">
-        <v>1.284903137564949</v>
+        <v>1.272630327577264</v>
       </c>
       <c r="P13" t="n">
-        <v>7.662493543578759</v>
+        <v>7.935681835074612</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.085346773752735</v>
+        <v>1.094914530019117</v>
       </c>
       <c r="R13" t="n">
-        <v>12.71690452994945</v>
+        <v>11.53579467546847</v>
       </c>
       <c r="S13" t="n">
-        <v>1.150093954081769</v>
+        <v>1.144181931031334</v>
       </c>
       <c r="T13" t="n">
-        <v>2.551211978700033</v>
+        <v>2.493765382457853</v>
       </c>
       <c r="U13" t="n">
-        <v>1.64465721882707</v>
+        <v>1.669449173038535</v>
       </c>
       <c r="V13" t="n">
-        <v>3.188207299953841</v>
+        <v>2.925078747206789</v>
       </c>
       <c r="W13" t="n">
-        <v>1.456995093664615</v>
+        <v>1.51945926962778</v>
       </c>
       <c r="X13" t="n">
-        <v>4.315231556463168</v>
+        <v>4.180687923311669</v>
       </c>
       <c r="Y13" t="n">
-        <v>1.301638055432497</v>
+        <v>1.31439739581833</v>
       </c>
       <c r="Z13" t="n">
-        <v>5.863046581706702</v>
+        <v>5.211713803815157</v>
       </c>
       <c r="AA13" t="n">
-        <v>1.205632412356833</v>
+        <v>1.23743303713898</v>
       </c>
       <c r="AB13" t="n">
-        <v>8.192055562825649</v>
+        <v>7.861472555895426</v>
       </c>
       <c r="AC13" t="n">
-        <v>1.139042307343787</v>
+        <v>1.14574131017121</v>
       </c>
       <c r="AD13" t="n">
-        <v>12.16410404151427</v>
+        <v>10.45695336808394</v>
       </c>
       <c r="AE13" t="n">
-        <v>1.08957279476091</v>
+        <v>1.105742299985837</v>
       </c>
     </row>
     <row r="14">
@@ -1848,85 +1848,85 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1.209107988436613</v>
+        <v>1.185135382972137</v>
       </c>
       <c r="F14" t="n">
-        <v>13.76577870776965</v>
+        <v>15.10504545588787</v>
       </c>
       <c r="G14" t="n">
-        <v>9.970079504989293</v>
+        <v>11.10969167740878</v>
       </c>
       <c r="H14" t="n">
-        <v>1.373371774096445</v>
+        <v>1.329485731516454</v>
       </c>
       <c r="I14" t="n">
-        <v>1.055818480942664</v>
+        <v>1.049624253878911</v>
       </c>
       <c r="J14" t="n">
-        <v>18.91521344027933</v>
+        <v>21.15143648184843</v>
       </c>
       <c r="K14" t="n">
-        <v>3.678295654297884</v>
+        <v>4.035032793066675</v>
       </c>
       <c r="L14" t="n">
-        <v>1.644066814925543</v>
+        <v>1.565376023130016</v>
       </c>
       <c r="M14" t="n">
-        <v>1.025959905363033</v>
+        <v>1.023140528297569</v>
       </c>
       <c r="N14" t="n">
-        <v>39.52094166044231</v>
+        <v>44.21422515254582</v>
       </c>
       <c r="O14" t="n">
-        <v>2.552633945463568</v>
+        <v>2.768734362776533</v>
       </c>
       <c r="P14" t="n">
-        <v>2.08954968083223</v>
+        <v>1.948773977136531</v>
       </c>
       <c r="Q14" t="n">
-        <v>1.011129228926067</v>
+        <v>1.009960611260003</v>
       </c>
       <c r="R14" t="n">
-        <v>90.85348460734588</v>
+        <v>101.3954450080252</v>
       </c>
       <c r="S14" t="n">
-        <v>1.91781037394841</v>
+        <v>2.053991808479056</v>
       </c>
       <c r="T14" t="n">
-        <v>1.283337418528626</v>
+        <v>1.227092636216611</v>
       </c>
       <c r="U14" t="n">
-        <v>4.529360877193731</v>
+        <v>5.403489327792016</v>
       </c>
       <c r="V14" t="n">
-        <v>4.833389705771483</v>
+        <v>4.53949139728145</v>
       </c>
       <c r="W14" t="n">
-        <v>1.260865728964216</v>
+        <v>1.282526467155158</v>
       </c>
       <c r="X14" t="n">
-        <v>1.575488024689801</v>
+        <v>1.46510483339801</v>
       </c>
       <c r="Y14" t="n">
-        <v>2.737655619400627</v>
+        <v>3.150052908919692</v>
       </c>
       <c r="Z14" t="n">
-        <v>10.25635402503918</v>
+        <v>9.435250636497589</v>
       </c>
       <c r="AA14" t="n">
-        <v>1.108033897287735</v>
+        <v>1.1185501229416</v>
       </c>
       <c r="AB14" t="n">
-        <v>2.093965076781798</v>
+        <v>1.883480759713229</v>
       </c>
       <c r="AC14" t="n">
-        <v>1.914105963000005</v>
+        <v>2.131886562333958</v>
       </c>
       <c r="AD14" t="n">
-        <v>24.72306273863493</v>
+        <v>22.25818055259501</v>
       </c>
       <c r="AE14" t="n">
-        <v>1.042153073193683</v>
+        <v>1.0470407143982</v>
       </c>
     </row>
     <row r="15">
@@ -1951,85 +1951,85 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>1.567876903472875</v>
+        <v>1.790521465122191</v>
       </c>
       <c r="F15" t="n">
-        <v>7.613527945879362</v>
+        <v>7.09970124094787</v>
       </c>
       <c r="G15" t="n">
-        <v>4.331823336084757</v>
+        <v>3.326099213919304</v>
       </c>
       <c r="H15" t="n">
-        <v>2.046738966575963</v>
+        <v>2.436706739072624</v>
       </c>
       <c r="I15" t="n">
-        <v>1.15143762728388</v>
+        <v>1.22664932103983</v>
       </c>
       <c r="J15" t="n">
-        <v>7.603378684251528</v>
+        <v>5.412102341238725</v>
       </c>
       <c r="K15" t="n">
-        <v>1.955348020787979</v>
+        <v>1.696036270175421</v>
       </c>
       <c r="L15" t="n">
-        <v>2.918941909316889</v>
+        <v>3.631088972036415</v>
       </c>
       <c r="M15" t="n">
-        <v>1.071621050656204</v>
+        <v>1.113750241032529</v>
       </c>
       <c r="N15" t="n">
-        <v>14.9623754585813</v>
+        <v>9.79119016296446</v>
       </c>
       <c r="O15" t="n">
-        <v>1.521120517064523</v>
+        <v>1.380070765613836</v>
       </c>
       <c r="P15" t="n">
-        <v>4.569431804507134</v>
+        <v>5.945667826354293</v>
       </c>
       <c r="Q15" t="n">
-        <v>1.031287280131874</v>
+        <v>1.053497835377221</v>
       </c>
       <c r="R15" t="n">
-        <v>32.9618706319329</v>
+        <v>19.69234508179359</v>
       </c>
       <c r="S15" t="n">
-        <v>1.280156634099942</v>
+        <v>1.202197162266183</v>
       </c>
       <c r="T15" t="n">
-        <v>2.259483823109361</v>
+        <v>2.433648191174552</v>
       </c>
       <c r="U15" t="n">
-        <v>1.793976057216235</v>
+        <v>1.697521195336441</v>
       </c>
       <c r="V15" t="n">
-        <v>5.903444965526613</v>
+        <v>4.247598464334214</v>
       </c>
       <c r="W15" t="n">
-        <v>1.203938253009964</v>
+        <v>1.307919840147174</v>
       </c>
       <c r="X15" t="n">
-        <v>3.641395563163178</v>
+        <v>4.040846440794581</v>
       </c>
       <c r="Y15" t="n">
-        <v>1.37858774881959</v>
+        <v>1.328855803629037</v>
       </c>
       <c r="Z15" t="n">
-        <v>13.35950594235079</v>
+        <v>8.634317610341641</v>
       </c>
       <c r="AA15" t="n">
-        <v>1.080909383001583</v>
+        <v>1.130987476686243</v>
       </c>
       <c r="AB15" t="n">
-        <v>6.563428832397946</v>
+        <v>7.520648777502621</v>
       </c>
       <c r="AC15" t="n">
-        <v>1.179745266835557</v>
+        <v>1.153358973028907</v>
       </c>
       <c r="AD15" t="n">
-        <v>34.42880524943437</v>
+        <v>19.90113945125158</v>
       </c>
       <c r="AE15" t="n">
-        <v>1.02991432067459</v>
+        <v>1.052906863238543</v>
       </c>
     </row>
     <row r="16">
@@ -2054,85 +2054,85 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>1.586495278406215</v>
+        <v>1.363923885202606</v>
       </c>
       <c r="F16" t="n">
-        <v>7.537340366629405</v>
+        <v>9.906185005115955</v>
       </c>
       <c r="G16" t="n">
-        <v>4.219284304326422</v>
+        <v>6.028664288951375</v>
       </c>
       <c r="H16" t="n">
-        <v>2.080255361250555</v>
+        <v>1.642738878777742</v>
       </c>
       <c r="I16" t="n">
-        <v>1.157275898661488</v>
+        <v>1.103252373710711</v>
       </c>
       <c r="J16" t="n">
-        <v>7.358253289350733</v>
+        <v>10.68500736653048</v>
       </c>
       <c r="K16" t="n">
-        <v>1.925707046565687</v>
+        <v>2.55584177808201</v>
       </c>
       <c r="L16" t="n">
-        <v>2.981502624941098</v>
+        <v>2.113401879656806</v>
       </c>
       <c r="M16" t="n">
-        <v>1.074737270284719</v>
+        <v>1.050248273934449</v>
       </c>
       <c r="N16" t="n">
-        <v>14.38020503278224</v>
+        <v>20.90118110931609</v>
       </c>
       <c r="O16" t="n">
-        <v>1.504667512125918</v>
+        <v>1.898148295122547</v>
       </c>
       <c r="P16" t="n">
-        <v>4.692417989205637</v>
+        <v>2.922204761589236</v>
       </c>
       <c r="Q16" t="n">
-        <v>1.032841377350513</v>
+        <v>1.022677101487431</v>
       </c>
       <c r="R16" t="n">
-        <v>31.44939282926833</v>
+        <v>45.0973464159097</v>
       </c>
       <c r="S16" t="n">
-        <v>1.270825243220943</v>
+        <v>1.520235939470477</v>
       </c>
       <c r="T16" t="n">
-        <v>2.287094708943788</v>
+        <v>1.517957604427166</v>
       </c>
       <c r="U16" t="n">
-        <v>1.776943602557901</v>
+        <v>2.930659944853879</v>
       </c>
       <c r="V16" t="n">
-        <v>5.76135660508616</v>
+        <v>4.35681776835258</v>
       </c>
       <c r="W16" t="n">
-        <v>1.210024176498728</v>
+        <v>1.297901187674769</v>
       </c>
       <c r="X16" t="n">
-        <v>3.704147177524069</v>
+        <v>2.044232403657739</v>
       </c>
       <c r="Y16" t="n">
-        <v>1.369802357028365</v>
+        <v>1.957641226701258</v>
       </c>
       <c r="Z16" t="n">
-        <v>12.93781542431235</v>
+        <v>8.93225904687143</v>
       </c>
       <c r="AA16" t="n">
-        <v>1.083767420123067</v>
+        <v>1.126067491504127</v>
       </c>
       <c r="AB16" t="n">
-        <v>6.712146686354352</v>
+        <v>3.023748182430139</v>
       </c>
       <c r="AC16" t="n">
-        <v>1.175065532261082</v>
+        <v>1.494132624148519</v>
       </c>
       <c r="AD16" t="n">
-        <v>33.07666439252557</v>
+        <v>20.77226497147352</v>
       </c>
       <c r="AE16" t="n">
-        <v>1.031175311365387</v>
+        <v>1.050575895146193</v>
       </c>
     </row>
     <row r="17">
@@ -2157,85 +2157,85 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>4.425628848499814</v>
+        <v>4.759270459486919</v>
       </c>
       <c r="F17" t="n">
-        <v>9.038913286717641</v>
+        <v>9.497247325585811</v>
       </c>
       <c r="G17" t="n">
-        <v>1.507362011038076</v>
+        <v>1.460728114988945</v>
       </c>
       <c r="H17" t="n">
-        <v>7.169843991175479</v>
+        <v>7.757180151156741</v>
       </c>
       <c r="I17" t="n">
-        <v>2.159121284735777</v>
+        <v>2.283535686458462</v>
       </c>
       <c r="J17" t="n">
-        <v>1.862722489155181</v>
+        <v>1.779097932804038</v>
       </c>
       <c r="K17" t="n">
-        <v>1.162078652463542</v>
+        <v>1.147990726550159</v>
       </c>
       <c r="L17" t="n">
-        <v>12.66390675315545</v>
+        <v>13.75940047451036</v>
       </c>
       <c r="M17" t="n">
-        <v>1.687089492900077</v>
+        <v>1.767065068137085</v>
       </c>
       <c r="N17" t="n">
-        <v>2.455414484333308</v>
+        <v>2.303670368445569</v>
       </c>
       <c r="O17" t="n">
-        <v>1.085734567427802</v>
+        <v>1.078373588320056</v>
       </c>
       <c r="P17" t="n">
-        <v>24.40002825144752</v>
+        <v>26.57388779493776</v>
       </c>
       <c r="Q17" t="n">
-        <v>1.404943771477477</v>
+        <v>1.457193623445761</v>
       </c>
       <c r="R17" t="n">
-        <v>3.469478654657168</v>
+        <v>3.187257102282475</v>
       </c>
       <c r="S17" t="n">
-        <v>1.042734991139942</v>
+        <v>1.03910238474566</v>
       </c>
       <c r="T17" t="n">
-        <v>2.818444823029776</v>
+        <v>2.737499397804152</v>
       </c>
       <c r="U17" t="n">
-        <v>1.549920452540245</v>
+        <v>1.575539767820235</v>
       </c>
       <c r="V17" t="n">
-        <v>1.476352489521448</v>
+        <v>1.401525376697351</v>
       </c>
       <c r="W17" t="n">
-        <v>3.099285764213422</v>
+        <v>3.490502613372176</v>
       </c>
       <c r="X17" t="n">
-        <v>4.952441321501208</v>
+        <v>4.757503329620183</v>
       </c>
       <c r="Y17" t="n">
-        <v>1.253008183716737</v>
+        <v>1.266134162042401</v>
       </c>
       <c r="Z17" t="n">
-        <v>1.959910070178522</v>
+        <v>1.809628312198106</v>
       </c>
       <c r="AA17" t="n">
-        <v>2.041764255909955</v>
+        <v>2.235134672211553</v>
       </c>
       <c r="AB17" t="n">
-        <v>9.791312240429161</v>
+        <v>9.296377995783509</v>
       </c>
       <c r="AC17" t="n">
-        <v>1.113748661479823</v>
+        <v>1.120534527297121</v>
       </c>
       <c r="AD17" t="n">
-        <v>2.852262880225011</v>
+        <v>2.551163197590005</v>
       </c>
       <c r="AE17" t="n">
-        <v>1.539880170723132</v>
+        <v>1.644677492061228</v>
       </c>
     </row>
     <row r="18">
@@ -2260,85 +2260,85 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>1.1764419695738</v>
+        <v>1.183935731833171</v>
       </c>
       <c r="F18" t="n">
-        <v>15.49708051096329</v>
+        <v>15.166829947791</v>
       </c>
       <c r="G18" t="n">
-        <v>11.70260780955664</v>
+        <v>11.1824049374413</v>
       </c>
       <c r="H18" t="n">
-        <v>1.316190028812062</v>
+        <v>1.327509685521211</v>
       </c>
       <c r="I18" t="n">
-        <v>1.046361835549002</v>
+        <v>1.049228700893391</v>
       </c>
       <c r="J18" t="n">
-        <v>22.56946523273572</v>
+        <v>21.31335342700951</v>
       </c>
       <c r="K18" t="n">
-        <v>4.162655077255404</v>
+        <v>4.053344814546667</v>
       </c>
       <c r="L18" t="n">
-        <v>1.545362514177303</v>
+        <v>1.562156958737098</v>
       </c>
       <c r="M18" t="n">
-        <v>1.021338126805855</v>
+        <v>1.022933455440054</v>
       </c>
       <c r="N18" t="n">
-        <v>47.86446983366951</v>
+        <v>44.60441899450787</v>
       </c>
       <c r="O18" t="n">
-        <v>2.833642712881602</v>
+        <v>2.778862619163389</v>
       </c>
       <c r="P18" t="n">
-        <v>1.918563979026671</v>
+        <v>1.943496324225437</v>
       </c>
       <c r="Q18" t="n">
-        <v>1.009048230098039</v>
+        <v>1.00986055891677</v>
       </c>
       <c r="R18" t="n">
-        <v>111.5188516610293</v>
+        <v>102.4141296087489</v>
       </c>
       <c r="S18" t="n">
-        <v>2.088655796256697</v>
+        <v>2.059887542032502</v>
       </c>
       <c r="T18" t="n">
-        <v>1.229357875951071</v>
+        <v>1.226178448410362</v>
       </c>
       <c r="U18" t="n">
-        <v>5.359998521321031</v>
+        <v>5.421287735539117</v>
       </c>
       <c r="V18" t="n">
-        <v>4.849271366489655</v>
+        <v>4.557132323490399</v>
       </c>
       <c r="W18" t="n">
-        <v>1.25978942630692</v>
+        <v>1.281125330479345</v>
       </c>
       <c r="X18" t="n">
-        <v>1.469542784393753</v>
+        <v>1.463313918603542</v>
       </c>
       <c r="Y18" t="n">
-        <v>3.129731375365813</v>
+        <v>3.158363821691487</v>
       </c>
       <c r="Z18" t="n">
-        <v>10.30112948495734</v>
+        <v>9.484128833838799</v>
       </c>
       <c r="AA18" t="n">
-        <v>1.107513824166978</v>
+        <v>1.117867139877876</v>
       </c>
       <c r="AB18" t="n">
-        <v>1.891882688007872</v>
+        <v>1.880091600080478</v>
       </c>
       <c r="AC18" t="n">
-        <v>2.121223691687099</v>
+        <v>2.136245363446893</v>
       </c>
       <c r="AD18" t="n">
-        <v>24.85881852925363</v>
+        <v>22.40356962275347</v>
       </c>
       <c r="AE18" t="n">
-        <v>1.041913223774006</v>
+        <v>1.046721178645684</v>
       </c>
     </row>
     <row r="19">
@@ -2363,85 +2363,85 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1.399990542550285</v>
+        <v>1.351422527197567</v>
       </c>
       <c r="F19" t="n">
-        <v>8.796859221647132</v>
+        <v>10.31391835759162</v>
       </c>
       <c r="G19" t="n">
-        <v>5.812854292369102</v>
+        <v>6.131861561289377</v>
       </c>
       <c r="H19" t="n">
-        <v>1.740128953774035</v>
+        <v>1.612271048653916</v>
       </c>
       <c r="I19" t="n">
-        <v>1.101733891642287</v>
+        <v>1.102889487443615</v>
       </c>
       <c r="J19" t="n">
-        <v>10.82956597705076</v>
+        <v>10.71916592108613</v>
       </c>
       <c r="K19" t="n">
-        <v>2.351115903385268</v>
+        <v>2.633263572070751</v>
       </c>
       <c r="L19" t="n">
-        <v>2.343597091044774</v>
+        <v>2.046139227677672</v>
       </c>
       <c r="M19" t="n">
-        <v>1.046168141501393</v>
+        <v>1.051076232491334</v>
       </c>
       <c r="N19" t="n">
-        <v>22.65995787311086</v>
+        <v>20.57857796519474</v>
       </c>
       <c r="O19" t="n">
-        <v>1.744270739096647</v>
+        <v>1.95589571019137</v>
       </c>
       <c r="P19" t="n">
-        <v>3.441429288583933</v>
+        <v>2.77916837522133</v>
       </c>
       <c r="Q19" t="n">
-        <v>1.019179872950635</v>
+        <v>1.023599158522498</v>
       </c>
       <c r="R19" t="n">
-        <v>53.13798874339766</v>
+        <v>43.37439224990318</v>
       </c>
       <c r="S19" t="n">
-        <v>1.409596134803484</v>
+        <v>1.562060350176581</v>
       </c>
       <c r="T19" t="n">
-        <v>1.923389692655602</v>
+        <v>1.425398587002292</v>
       </c>
       <c r="U19" t="n">
-        <v>2.08296638781409</v>
+        <v>3.350736534051091</v>
       </c>
       <c r="V19" t="n">
-        <v>7.079511263003193</v>
+        <v>3.797057236032786</v>
       </c>
       <c r="W19" t="n">
-        <v>1.164486906387606</v>
+        <v>1.357518604595433</v>
       </c>
       <c r="X19" t="n">
-        <v>2.895790733637381</v>
+        <v>1.857388431358307</v>
       </c>
       <c r="Y19" t="n">
-        <v>1.527484380135849</v>
+        <v>2.166332508610785</v>
       </c>
       <c r="Z19" t="n">
-        <v>16.95204170770465</v>
+        <v>7.428440559930785</v>
       </c>
       <c r="AA19" t="n">
-        <v>1.062687900290344</v>
+        <v>1.155558722317994</v>
       </c>
       <c r="AB19" t="n">
-        <v>4.848014056285145</v>
+        <v>2.646215606019505</v>
       </c>
       <c r="AC19" t="n">
-        <v>1.259874310585392</v>
+        <v>1.607453845257832</v>
       </c>
       <c r="AD19" t="n">
-        <v>46.31575200177343</v>
+        <v>16.44879096990615</v>
       </c>
       <c r="AE19" t="n">
-        <v>1.022067381778435</v>
+        <v>1.064729984498332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>